<commit_message>
Minor corrections on the 'Analysis Services' sheet
</commit_message>
<xml_diff>
--- a/configuration/senaite/configuration.xlsx
+++ b/configuration/senaite/configuration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="0" windowWidth="25040" windowHeight="16600" tabRatio="950" firstSheet="2" activeTab="10"/>
+    <workbookView xWindow="600" yWindow="0" windowWidth="27520" windowHeight="15500" tabRatio="950" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Lab Departments" sheetId="12" r:id="rId1"/>
@@ -22,7 +22,6 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId13"/>
-    <externalReference r:id="rId14"/>
   </externalReferences>
   <calcPr calcId="140000" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -827,9 +826,6 @@
     <t>VERY LOW DENSITY LIPOPROTEIN</t>
   </si>
   <si>
-    <t>Very Low Density Lipoprotein (VLDL) is one of three major lipoprotein particles.  VLDL contains the highest amount of triglyceride. Since VLDL contains most of the circulating triglyceride and since the compositions of the different particles are relatively constant, it is possible to estimate the amount of VLDL cholesterol by dividing the triglyceride value (in mg/dL) by 5 (1298AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA)</t>
-  </si>
-  <si>
     <t>HIGH-DENSITY LIPOPROTEIN CHOLESTEROL</t>
   </si>
   <si>
@@ -1767,6 +1763,9 @@
   </si>
   <si>
     <t>Different type water samples</t>
+  </si>
+  <si>
+    <t>Very Low Density Lipoprotein {VLDL} is one of three major lipoprotein particles.  VLDL contains the highest amount of triglyceride. Since VLDL contains most of the circulating triglyceride and since the compositions of the different particles are relatively constant, it is possible to estimate the amount of VLDL cholesterol by dividing the triglyceride value (in mg/dL) by 5 (1298AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA)</t>
   </si>
 </sst>
 </file>
@@ -1958,7 +1957,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1978,6 +1977,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2146,9 +2148,6 @@
     <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -2190,8 +2189,11 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="44">
+  <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2225,6 +2227,9 @@
     <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2368,137 +2373,6 @@
       <sheetData sheetId="57"/>
       <sheetData sheetId="58"/>
       <sheetData sheetId="59"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Instructions"/>
-      <sheetName val="Lab Information"/>
-      <sheetName val="Lab Contacts"/>
-      <sheetName val="Lab Departments"/>
-      <sheetName val="Lab Products"/>
-      <sheetName val="Clients"/>
-      <sheetName val="Client Contacts"/>
-      <sheetName val="Attachment Types"/>
-      <sheetName val="Container Types"/>
-      <sheetName val="Preservations"/>
-      <sheetName val="Storage Locations"/>
-      <sheetName val="Supply Orders"/>
-      <sheetName val="Containers"/>
-      <sheetName val="Sample Matrices"/>
-      <sheetName val="Sample Types"/>
-      <sheetName val="Sample Points"/>
-      <sheetName val="Sample Point Sample Types"/>
-      <sheetName val="Methods"/>
-      <sheetName val="Manufacturers"/>
-      <sheetName val="Suppliers"/>
-      <sheetName val="Supplier Contacts"/>
-      <sheetName val="Instrument Types"/>
-      <sheetName val="Instruments"/>
-      <sheetName val="Instrument Validations"/>
-      <sheetName val="Instrument Calibrations"/>
-      <sheetName val="Instrument Documents"/>
-      <sheetName val="Instrument Certifications"/>
-      <sheetName val="Instrument Maintenance Tasks"/>
-      <sheetName val="Instrument Schedule"/>
-      <sheetName val="Analysis Categories"/>
-      <sheetName val="Calculations"/>
-      <sheetName val="Calculation Interim Fields"/>
-      <sheetName val="Analysis Services"/>
-      <sheetName val="AnalysisService Methods"/>
-      <sheetName val="AnalysisService Instruments"/>
-      <sheetName val="AnalysisService InterimFields"/>
-      <sheetName val="AnalysisService ResultOptions"/>
-      <sheetName val="Analysis Service Uncertainties"/>
-      <sheetName val="Analysis Profiles"/>
-      <sheetName val="Analysis Profile Services"/>
-      <sheetName val="Analysis Specifications"/>
-      <sheetName val="AR Templates"/>
-      <sheetName val="AR Template Analyses"/>
-      <sheetName val="AR Template Partitions"/>
-      <sheetName val="Reference Definitions"/>
-      <sheetName val="Reference Definition Results"/>
-      <sheetName val="Reference Samples"/>
-      <sheetName val="Reference Sample Results"/>
-      <sheetName val="Reference Analyses"/>
-      <sheetName val="Reference Analyses Interims"/>
-      <sheetName val="Sample Conditions"/>
-      <sheetName val="Sampling Deviations"/>
-      <sheetName val="Analysis Requests"/>
-      <sheetName val="Analyses"/>
-      <sheetName val="Analysis Interims"/>
-      <sheetName val="Worksheet Templates"/>
-      <sheetName val="Worksheet Template Services"/>
-      <sheetName val="Worksheet Template Layouts"/>
-      <sheetName val="Setup"/>
-      <sheetName val="Constants"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
-      <sheetData sheetId="34" refreshError="1"/>
-      <sheetData sheetId="35" refreshError="1"/>
-      <sheetData sheetId="36" refreshError="1"/>
-      <sheetData sheetId="37" refreshError="1"/>
-      <sheetData sheetId="38" refreshError="1"/>
-      <sheetData sheetId="39" refreshError="1"/>
-      <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41" refreshError="1"/>
-      <sheetData sheetId="42" refreshError="1"/>
-      <sheetData sheetId="43" refreshError="1"/>
-      <sheetData sheetId="44" refreshError="1"/>
-      <sheetData sheetId="45" refreshError="1"/>
-      <sheetData sheetId="46" refreshError="1"/>
-      <sheetData sheetId="47" refreshError="1"/>
-      <sheetData sheetId="48" refreshError="1"/>
-      <sheetData sheetId="49" refreshError="1"/>
-      <sheetData sheetId="50" refreshError="1"/>
-      <sheetData sheetId="51" refreshError="1"/>
-      <sheetData sheetId="52" refreshError="1"/>
-      <sheetData sheetId="53" refreshError="1"/>
-      <sheetData sheetId="54" refreshError="1"/>
-      <sheetData sheetId="55" refreshError="1"/>
-      <sheetData sheetId="56" refreshError="1"/>
-      <sheetData sheetId="57" refreshError="1"/>
-      <sheetData sheetId="58" refreshError="1"/>
-      <sheetData sheetId="59" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2999,7 +2873,7 @@
   <dimension ref="A1:AMJ9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3082,18 +2956,18 @@
     </row>
     <row r="4" spans="1:1024" ht="13.5" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="9" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>189</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="H4" s="10">
         <v>0</v>
@@ -3101,11 +2975,11 @@
     </row>
     <row r="5" spans="1:1024" ht="13.5" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="9" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>189</v>
@@ -3120,11 +2994,11 @@
     </row>
     <row r="6" spans="1:1024">
       <c r="A6" s="9" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>189</v>
@@ -3139,11 +3013,11 @@
     </row>
     <row r="7" spans="1:1024">
       <c r="A7" s="9" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="9" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>189</v>
@@ -3158,11 +3032,11 @@
     </row>
     <row r="8" spans="1:1024">
       <c r="A8" s="19" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>189</v>
@@ -3174,11 +3048,11 @@
     </row>
     <row r="9" spans="1:1024">
       <c r="A9" s="19" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="9" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>189</v>
@@ -3193,7 +3067,6 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
@@ -3255,8 +3128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3298,219 +3171,219 @@
     </row>
     <row r="4" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="C4" s="67" t="s">
+      <c r="C4" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="C5" s="67" t="s">
+      <c r="C5" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="C6" s="67" t="s">
+      <c r="C6" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="C7" s="67" t="s">
+      <c r="C7" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="C8" s="67" t="s">
+      <c r="C8" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="C9" s="67" t="s">
+      <c r="C9" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="C10" s="67" t="s">
+      <c r="C10" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="C11" s="67" t="s">
+      <c r="C11" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="C12" s="67" t="s">
+      <c r="C12" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="C13" s="67" t="s">
+      <c r="C13" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A14" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>548</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>549</v>
-      </c>
-      <c r="C14" s="67" t="s">
+      <c r="C14" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="C15" s="67" t="s">
+      <c r="C15" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="C16" s="67" t="s">
+      <c r="C16" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="C17" s="67" t="s">
+      <c r="C17" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="C18" s="67" t="s">
+      <c r="C18" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A19" s="9" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="C19" s="67" t="s">
+      <c r="C19" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C20" s="67" t="s">
+        <v>256</v>
+      </c>
+      <c r="C20" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A21" s="9" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="C21" s="67" t="s">
+      <c r="C21" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="C22" s="67" t="s">
+      <c r="C22" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A23" s="9" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>24</v>
@@ -3518,51 +3391,51 @@
     </row>
     <row r="24" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>271</v>
-      </c>
-      <c r="C24" s="67" t="s">
+        <v>270</v>
+      </c>
+      <c r="C24" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A25" s="9" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="C25" s="67" t="s">
+        <v>261</v>
+      </c>
+      <c r="C25" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>265</v>
-      </c>
-      <c r="C26" s="67" t="s">
+        <v>264</v>
+      </c>
+      <c r="C26" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A27" s="9" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="C27" s="67" t="s">
+        <v>260</v>
+      </c>
+      <c r="C27" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="13.5" customHeight="1">
       <c r="A28" s="19" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>244</v>
@@ -3573,7 +3446,7 @@
     </row>
     <row r="29" spans="1:3" ht="13.5" customHeight="1">
       <c r="A29" s="19" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>246</v>
@@ -3587,7 +3460,6 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
@@ -3641,35 +3513,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="28" customFormat="1" ht="44.75" customHeight="1">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="61" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="61" t="s">
         <v>125</v>
       </c>
       <c r="C1" s="39" t="s">
+        <v>273</v>
+      </c>
+      <c r="D1" s="39" t="s">
         <v>274</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="E1" s="39" t="s">
         <v>275</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="F1" s="28" t="s">
         <v>276</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="G1" s="61" t="s">
         <v>277</v>
       </c>
-      <c r="G1" s="62" t="s">
+      <c r="H1" s="39" t="s">
         <v>278</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="I1" s="39" t="s">
         <v>279</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="J1" s="39" t="s">
         <v>280</v>
-      </c>
-      <c r="J1" s="39" t="s">
-        <v>281</v>
       </c>
       <c r="K1" s="39" t="s">
         <v>66</v>
@@ -3678,1202 +3550,1202 @@
     </row>
     <row r="2" spans="1:12" ht="13.5" customHeight="1">
       <c r="A2" s="43" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B2" s="43" t="s">
         <v>168</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="62" t="s">
+        <v>282</v>
+      </c>
+      <c r="D2" s="62" t="s">
         <v>283</v>
       </c>
-      <c r="D2" s="63" t="s">
+      <c r="E2" s="62" t="s">
         <v>284</v>
       </c>
-      <c r="E2" s="63" t="s">
+      <c r="F2" s="62" t="s">
         <v>285</v>
       </c>
-      <c r="F2" s="63" t="s">
+      <c r="G2" s="62">
+        <v>0</v>
+      </c>
+      <c r="H2" s="62" t="s">
         <v>286</v>
       </c>
-      <c r="G2" s="63">
-        <v>0</v>
-      </c>
-      <c r="H2" s="63" t="s">
+      <c r="I2" s="62" t="s">
         <v>287</v>
       </c>
-      <c r="I2" s="63" t="s">
+      <c r="J2" s="62" t="s">
         <v>288</v>
       </c>
-      <c r="J2" s="63" t="s">
-        <v>289</v>
-      </c>
-      <c r="K2" s="63" t="s">
+      <c r="K2" s="62" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="13.5" customHeight="1">
       <c r="A3" s="43" t="s">
+        <v>289</v>
+      </c>
+      <c r="B3" s="43" t="s">
         <v>290</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="C3" s="62" t="s">
         <v>291</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="D3" s="62" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="62" t="s">
         <v>292</v>
       </c>
-      <c r="D3" s="63" t="s">
-        <v>88</v>
-      </c>
-      <c r="E3" s="63" t="s">
+      <c r="F3" s="62" t="s">
         <v>293</v>
       </c>
-      <c r="F3" s="63" t="s">
+      <c r="G3" s="62">
+        <v>1</v>
+      </c>
+      <c r="H3" s="62" t="s">
         <v>294</v>
       </c>
-      <c r="G3" s="63">
-        <v>1</v>
-      </c>
-      <c r="H3" s="63" t="s">
+      <c r="I3" s="62" t="s">
         <v>295</v>
       </c>
-      <c r="I3" s="63" t="s">
+      <c r="J3" s="62" t="s">
         <v>296</v>
       </c>
-      <c r="J3" s="63" t="s">
-        <v>297</v>
-      </c>
-      <c r="K3" s="63" t="s">
+      <c r="K3" s="62" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="24.5" customHeight="1">
       <c r="A4" s="43" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B4" s="43" t="s">
         <v>158</v>
       </c>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="62" t="s">
+        <v>298</v>
+      </c>
+      <c r="D4" s="62" t="s">
         <v>299</v>
       </c>
-      <c r="D4" s="63" t="s">
+      <c r="F4" s="62" t="s">
         <v>300</v>
       </c>
-      <c r="F4" s="63" t="s">
+      <c r="G4" s="62"/>
+      <c r="H4" s="62" t="s">
         <v>301</v>
       </c>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63" t="s">
-        <v>302</v>
-      </c>
     </row>
     <row r="5" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="62" t="s">
         <v>179</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="62" t="s">
         <v>180</v>
       </c>
-      <c r="G5" s="63"/>
+      <c r="G5" s="62"/>
     </row>
     <row r="6" spans="1:12" ht="13.5" customHeight="1">
       <c r="A6" s="43" t="s">
+        <v>302</v>
+      </c>
+      <c r="B6" s="43" t="s">
         <v>303</v>
       </c>
-      <c r="B6" s="43" t="s">
-        <v>304</v>
-      </c>
-      <c r="G6" s="63"/>
+      <c r="G6" s="62"/>
     </row>
     <row r="7" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A7" s="63" t="s">
+      <c r="A7" s="62" t="s">
         <v>177</v>
       </c>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="62" t="s">
         <v>178</v>
       </c>
-      <c r="G7" s="63"/>
+      <c r="G7" s="62"/>
     </row>
     <row r="8" spans="1:12" ht="13.5" customHeight="1">
       <c r="A8" s="43" t="s">
+        <v>304</v>
+      </c>
+      <c r="B8" s="43" t="s">
         <v>305</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="G8" s="62"/>
+    </row>
+    <row r="9" spans="1:12" ht="13.5" customHeight="1">
+      <c r="G9" s="62"/>
+    </row>
+    <row r="10" spans="1:12" ht="13.5" customHeight="1">
+      <c r="G10" s="62"/>
+    </row>
+    <row r="11" spans="1:12" ht="13.5" customHeight="1">
+      <c r="G11" s="62"/>
+    </row>
+    <row r="12" spans="1:12" ht="13.5" customHeight="1">
+      <c r="G12" s="62"/>
+    </row>
+    <row r="13" spans="1:12" ht="13.5" customHeight="1">
+      <c r="G13" s="62"/>
+    </row>
+    <row r="14" spans="1:12" ht="13.5" customHeight="1">
+      <c r="G14" s="62"/>
+    </row>
+    <row r="15" spans="1:12" ht="13.5" customHeight="1">
+      <c r="G15" s="62"/>
+    </row>
+    <row r="16" spans="1:12" ht="13.5" customHeight="1">
+      <c r="G16" s="62"/>
+    </row>
+    <row r="17" spans="1:12" ht="13.5" customHeight="1">
+      <c r="G17" s="62"/>
+    </row>
+    <row r="18" spans="1:12" ht="13.5" customHeight="1">
+      <c r="G18" s="62"/>
+    </row>
+    <row r="19" spans="1:12" ht="13.5" customHeight="1">
+      <c r="G19" s="62"/>
+    </row>
+    <row r="20" spans="1:12" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A20" s="63"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="63"/>
+      <c r="J20" s="63"/>
+      <c r="K20" s="63"/>
+      <c r="L20" s="63"/>
+    </row>
+    <row r="21" spans="1:12" s="64" customFormat="1" ht="69.75" customHeight="1" thickTop="1">
+      <c r="A21" s="28" t="s">
         <v>306</v>
       </c>
-      <c r="G8" s="63"/>
-    </row>
-    <row r="9" spans="1:12" ht="13.5" customHeight="1">
-      <c r="G9" s="63"/>
-    </row>
-    <row r="10" spans="1:12" ht="13.5" customHeight="1">
-      <c r="G10" s="63"/>
-    </row>
-    <row r="11" spans="1:12" ht="13.5" customHeight="1">
-      <c r="G11" s="63"/>
-    </row>
-    <row r="12" spans="1:12" ht="13.5" customHeight="1">
-      <c r="G12" s="63"/>
-    </row>
-    <row r="13" spans="1:12" ht="13.5" customHeight="1">
-      <c r="G13" s="63"/>
-    </row>
-    <row r="14" spans="1:12" ht="13.5" customHeight="1">
-      <c r="G14" s="63"/>
-    </row>
-    <row r="15" spans="1:12" ht="13.5" customHeight="1">
-      <c r="G15" s="63"/>
-    </row>
-    <row r="16" spans="1:12" ht="13.5" customHeight="1">
-      <c r="G16" s="63"/>
-    </row>
-    <row r="17" spans="1:12" ht="13.5" customHeight="1">
-      <c r="G17" s="63"/>
-    </row>
-    <row r="18" spans="1:12" ht="13.5" customHeight="1">
-      <c r="G18" s="63"/>
-    </row>
-    <row r="19" spans="1:12" ht="13.5" customHeight="1">
-      <c r="G19" s="63"/>
-    </row>
-    <row r="20" spans="1:12" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A20" s="64"/>
-      <c r="B20" s="64"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="64"/>
-      <c r="H20" s="64"/>
-      <c r="I20" s="64"/>
-      <c r="J20" s="64"/>
-      <c r="K20" s="64"/>
-      <c r="L20" s="64"/>
-    </row>
-    <row r="21" spans="1:12" s="65" customFormat="1" ht="69.75" customHeight="1" thickTop="1">
-      <c r="A21" s="28" t="s">
+      <c r="B21" s="39" t="s">
         <v>307</v>
       </c>
-      <c r="B21" s="39" t="s">
+      <c r="C21" s="28" t="s">
         <v>308</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="D21" s="28" t="s">
         <v>309</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="E21" s="28" t="s">
         <v>310</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="F21" s="28" t="s">
         <v>311</v>
       </c>
-      <c r="F21" s="28" t="s">
+      <c r="G21" s="28" t="s">
         <v>312</v>
       </c>
-      <c r="G21" s="28" t="s">
+      <c r="H21" s="28" t="s">
         <v>313</v>
       </c>
-      <c r="H21" s="28" t="s">
+      <c r="I21" s="28" t="s">
         <v>314</v>
       </c>
-      <c r="I21" s="28" t="s">
+    </row>
+    <row r="22" spans="1:12" ht="13.5" customHeight="1">
+      <c r="A22" s="65" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A22" s="66" t="s">
+      <c r="B22" s="62" t="s">
         <v>316</v>
       </c>
-      <c r="B22" s="63" t="s">
+      <c r="C22" s="62" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="62" t="s">
         <v>317</v>
       </c>
-      <c r="C22" s="63" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="63" t="s">
+      <c r="E22" s="62" t="s">
         <v>318</v>
       </c>
-      <c r="E22" s="63" t="s">
+      <c r="F22" s="62" t="s">
         <v>319</v>
       </c>
-      <c r="F22" s="63" t="s">
+      <c r="G22" s="62" t="s">
         <v>320</v>
       </c>
-      <c r="G22" s="63" t="s">
+      <c r="H22" s="62" t="s">
+        <v>320</v>
+      </c>
+      <c r="I22" s="62" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="24.5" customHeight="1">
+      <c r="B23" s="62" t="s">
         <v>321</v>
       </c>
-      <c r="H22" s="63" t="s">
-        <v>321</v>
-      </c>
-      <c r="I22" s="63" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="24.5" customHeight="1">
-      <c r="B23" s="63" t="s">
+      <c r="C23" s="62" t="s">
         <v>322</v>
       </c>
-      <c r="C23" s="63" t="s">
+      <c r="D23" s="62" t="s">
         <v>323</v>
       </c>
-      <c r="D23" s="63" t="s">
+      <c r="E23" s="62" t="s">
         <v>324</v>
       </c>
-      <c r="E23" s="63" t="s">
+      <c r="F23" s="62" t="s">
         <v>325</v>
       </c>
-      <c r="F23" s="63" t="s">
+      <c r="G23" s="62" t="s">
         <v>326</v>
       </c>
-      <c r="G23" s="63" t="s">
+      <c r="H23" s="62" t="s">
+        <v>326</v>
+      </c>
+      <c r="I23" s="62" t="s">
         <v>327</v>
       </c>
-      <c r="H23" s="63" t="s">
-        <v>327</v>
-      </c>
-      <c r="I23" s="63" t="s">
+    </row>
+    <row r="24" spans="1:12" ht="24.5" customHeight="1">
+      <c r="B24" s="62" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" ht="24.5" customHeight="1">
-      <c r="B24" s="63" t="s">
+      <c r="C24" s="62" t="s">
         <v>329</v>
       </c>
-      <c r="C24" s="63" t="s">
+      <c r="D24" s="62" t="s">
         <v>330</v>
       </c>
-      <c r="D24" s="63" t="s">
+      <c r="F24" s="62" t="s">
         <v>331</v>
       </c>
-      <c r="F24" s="63" t="s">
+      <c r="G24" s="62" t="s">
         <v>332</v>
       </c>
-      <c r="G24" s="63" t="s">
+      <c r="H24" s="62" t="s">
+        <v>332</v>
+      </c>
+      <c r="I24" s="62" t="s">
         <v>333</v>
       </c>
-      <c r="H24" s="63" t="s">
-        <v>333</v>
-      </c>
-      <c r="I24" s="63" t="s">
+    </row>
+    <row r="25" spans="1:12" ht="13.5" customHeight="1">
+      <c r="B25" s="62" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" ht="13.5" customHeight="1">
-      <c r="B25" s="63" t="s">
+      <c r="C25" s="62" t="s">
         <v>335</v>
       </c>
-      <c r="C25" s="63" t="s">
+      <c r="D25" s="62" t="s">
         <v>336</v>
       </c>
-      <c r="D25" s="63" t="s">
+      <c r="H25" s="62" t="s">
         <v>337</v>
       </c>
-      <c r="H25" s="63" t="s">
+      <c r="I25" s="62" t="s">
         <v>338</v>
       </c>
-      <c r="I25" s="63" t="s">
+    </row>
+    <row r="26" spans="1:12" ht="13.5" customHeight="1">
+      <c r="B26" s="62" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" ht="13.5" customHeight="1">
-      <c r="B26" s="63" t="s">
+      <c r="C26" s="62" t="s">
         <v>340</v>
       </c>
-      <c r="C26" s="63" t="s">
+      <c r="H26" s="62" t="s">
         <v>341</v>
       </c>
-      <c r="H26" s="63" t="s">
+    </row>
+    <row r="27" spans="1:12" ht="13.5" customHeight="1">
+      <c r="B27" s="62" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" ht="13.5" customHeight="1">
-      <c r="B27" s="63" t="s">
+      <c r="C27" s="62" t="s">
         <v>343</v>
       </c>
-      <c r="C27" s="63" t="s">
+    </row>
+    <row r="28" spans="1:12" ht="13.5" customHeight="1">
+      <c r="B28" s="62" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" ht="13.5" customHeight="1">
-      <c r="B28" s="63" t="s">
+      <c r="C28" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="C28" s="63" t="s">
+    </row>
+    <row r="29" spans="1:12" ht="13.5" customHeight="1">
+      <c r="B29" s="62" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" ht="13.5" customHeight="1">
-      <c r="B29" s="63" t="s">
+      <c r="C29" s="62" t="s">
         <v>347</v>
       </c>
-      <c r="C29" s="63" t="s">
+    </row>
+    <row r="30" spans="1:12" ht="13.5" customHeight="1">
+      <c r="B30" s="62" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" ht="13.5" customHeight="1">
-      <c r="B30" s="63" t="s">
+      <c r="C30" s="62" t="s">
         <v>349</v>
       </c>
-      <c r="C30" s="63" t="s">
+    </row>
+    <row r="31" spans="1:12" ht="13.5" customHeight="1">
+      <c r="B31" s="62" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" ht="13.5" customHeight="1">
-      <c r="B31" s="63" t="s">
+      <c r="C31" s="62" t="s">
         <v>351</v>
       </c>
-      <c r="C31" s="63" t="s">
+    </row>
+    <row r="32" spans="1:12" ht="13.5" customHeight="1">
+      <c r="B32" s="62" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" ht="13.5" customHeight="1">
-      <c r="B32" s="63" t="s">
+      <c r="C32" s="62" t="s">
         <v>353</v>
       </c>
-      <c r="C32" s="63" t="s">
+    </row>
+    <row r="33" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B33" s="62" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="33" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B33" s="63" t="s">
+      <c r="C33" s="62" t="s">
         <v>355</v>
       </c>
-      <c r="C33" s="63" t="s">
+    </row>
+    <row r="34" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B34" s="62" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="34" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B34" s="63" t="s">
+    <row r="35" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B35" s="62" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="35" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B35" s="63" t="s">
+    <row r="36" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B36" s="62" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="36" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B36" s="63" t="s">
+    <row r="37" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B37" s="62" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="37" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B37" s="63" t="s">
+    <row r="38" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B38" s="62" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="38" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B38" s="63" t="s">
+    <row r="39" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B39" s="62" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="39" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B39" s="63" t="s">
+    <row r="40" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B40" s="62" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="40" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B40" s="63" t="s">
+    <row r="41" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B41" s="62" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="41" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B41" s="63" t="s">
+    <row r="42" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B42" s="62" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="42" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B42" s="63" t="s">
+    <row r="43" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B43" s="62" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="43" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B43" s="63" t="s">
+    <row r="44" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B44" s="62" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="44" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B44" s="63" t="s">
+    <row r="45" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B45" s="62" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="45" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B45" s="63" t="s">
+    <row r="46" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B46" s="62" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="46" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B46" s="63" t="s">
+    <row r="47" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B47" s="62" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="47" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B47" s="63" t="s">
+    <row r="48" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B48" s="62" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="48" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B48" s="63" t="s">
+    <row r="49" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B49" s="62" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="49" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B49" s="63" t="s">
+    <row r="50" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B50" s="62" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="50" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B50" s="63" t="s">
+    <row r="51" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B51" s="62" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="51" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B51" s="63" t="s">
+    <row r="52" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B52" s="62" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="52" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B52" s="63" t="s">
+    <row r="53" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B53" s="62" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="53" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B53" s="63" t="s">
+    <row r="54" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B54" s="62" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="54" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B54" s="63" t="s">
+    <row r="55" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B55" s="62" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="55" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B55" s="63" t="s">
+    <row r="56" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B56" s="62" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="56" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B56" s="63" t="s">
+    <row r="57" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B57" s="62" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="57" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B57" s="63" t="s">
+    <row r="58" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B58" s="62" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="58" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B58" s="63" t="s">
+    <row r="59" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B59" s="62" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="59" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B59" s="63" t="s">
+    <row r="60" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B60" s="62" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="60" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B60" s="63" t="s">
+    <row r="61" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B61" s="62" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="61" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B61" s="63" t="s">
+    <row r="62" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B62" s="62" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="62" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B62" s="63" t="s">
+    <row r="63" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B63" s="62" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="63" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B63" s="63" t="s">
+    <row r="64" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B64" s="62" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="64" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B64" s="63" t="s">
+    <row r="65" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B65" s="62" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="65" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B65" s="63" t="s">
+    <row r="66" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B66" s="62" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="66" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B66" s="63" t="s">
+    <row r="67" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B67" s="62" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="67" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B67" s="63" t="s">
+    <row r="68" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B68" s="62" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="68" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B68" s="63" t="s">
+    <row r="69" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B69" s="62" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="69" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B69" s="63" t="s">
+    <row r="70" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B70" s="62" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="70" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B70" s="63" t="s">
+    <row r="71" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B71" s="62" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="71" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B71" s="63" t="s">
+    <row r="72" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B72" s="62" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="72" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B72" s="63" t="s">
+    <row r="73" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B73" s="62" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="73" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B73" s="63" t="s">
+    <row r="74" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B74" s="62" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="74" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B74" s="63" t="s">
+    <row r="75" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B75" s="62" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="75" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B75" s="63" t="s">
+    <row r="76" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B76" s="62" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="76" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B76" s="63" t="s">
+    <row r="77" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B77" s="62" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="77" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B77" s="63" t="s">
+    <row r="78" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B78" s="62" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="78" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B78" s="63" t="s">
+    <row r="79" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B79" s="62" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="79" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B79" s="63" t="s">
+    <row r="80" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B80" s="62" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="80" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B80" s="63" t="s">
+    <row r="81" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B81" s="62" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="81" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B81" s="63" t="s">
+    <row r="82" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B82" s="62" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="82" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B82" s="63" t="s">
+    <row r="83" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B83" s="62" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="83" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B83" s="63" t="s">
+    <row r="84" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B84" s="62" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="84" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B84" s="63" t="s">
+    <row r="85" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B85" s="62" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="85" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B85" s="63" t="s">
+    <row r="86" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B86" s="62" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="86" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B86" s="63" t="s">
+    <row r="87" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B87" s="62" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="87" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B87" s="63" t="s">
+    <row r="88" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B88" s="62" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="88" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B88" s="63" t="s">
+    <row r="89" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B89" s="62" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="89" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B89" s="63" t="s">
+    <row r="90" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B90" s="62" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="90" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B90" s="63" t="s">
+    <row r="91" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B91" s="62" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="91" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B91" s="63" t="s">
+    <row r="92" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B92" s="62" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="92" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B92" s="63" t="s">
+    <row r="93" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B93" s="62" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="93" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B93" s="63" t="s">
+    <row r="94" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B94" s="62" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="94" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B94" s="63" t="s">
+    <row r="95" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B95" s="62" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="95" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B95" s="63" t="s">
+    <row r="96" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B96" s="62" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="96" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B96" s="63" t="s">
+    <row r="97" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B97" s="62" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="97" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B97" s="63" t="s">
+    <row r="98" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B98" s="62" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="98" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B98" s="63" t="s">
+    <row r="99" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B99" s="62" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="99" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B99" s="63" t="s">
+    <row r="100" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B100" s="62" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="100" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B100" s="63" t="s">
+    <row r="101" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B101" s="62" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="101" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B101" s="63" t="s">
+    <row r="102" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B102" s="62" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="102" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B102" s="63" t="s">
+    <row r="103" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B103" s="62" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="103" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B103" s="63" t="s">
+    <row r="104" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B104" s="62" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="104" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B104" s="63" t="s">
+    <row r="105" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B105" s="62" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="105" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B105" s="63" t="s">
+    <row r="106" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B106" s="62" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="106" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B106" s="63" t="s">
+    <row r="107" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B107" s="62" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="107" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B107" s="63" t="s">
+    <row r="108" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B108" s="62" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="108" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B108" s="63" t="s">
+    <row r="109" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B109" s="62" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="109" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B109" s="63" t="s">
+    <row r="110" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B110" s="62" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="110" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B110" s="63" t="s">
+    <row r="111" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B111" s="62" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="111" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B111" s="63" t="s">
+    <row r="112" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B112" s="62" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="112" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B112" s="63" t="s">
+    <row r="113" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B113" s="62" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="113" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B113" s="63" t="s">
+    <row r="114" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B114" s="62" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="114" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B114" s="63" t="s">
+    <row r="115" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B115" s="62" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="115" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B115" s="63" t="s">
+    <row r="116" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B116" s="62" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="116" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B116" s="63" t="s">
+    <row r="117" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B117" s="62" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="117" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B117" s="63" t="s">
+    <row r="118" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B118" s="62" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="118" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B118" s="63" t="s">
+    <row r="119" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B119" s="62" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="119" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B119" s="63" t="s">
+    <row r="120" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B120" s="62" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="120" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B120" s="63" t="s">
+    <row r="121" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B121" s="62" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="121" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B121" s="63" t="s">
+    <row r="122" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B122" s="62" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="122" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B122" s="63" t="s">
+    <row r="123" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B123" s="62" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="123" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B123" s="63" t="s">
+    <row r="124" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B124" s="62" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="124" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B124" s="63" t="s">
+    <row r="125" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B125" s="62" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="125" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B125" s="63" t="s">
+    <row r="126" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B126" s="62" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="126" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B126" s="63" t="s">
+    <row r="127" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B127" s="62" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="127" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B127" s="63" t="s">
+    <row r="128" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B128" s="62" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="128" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B128" s="63" t="s">
+    <row r="129" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B129" s="62" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="129" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B129" s="63" t="s">
+    <row r="130" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B130" s="62" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="130" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B130" s="63" t="s">
+    <row r="131" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B131" s="62" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="131" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B131" s="63" t="s">
+    <row r="132" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B132" s="62" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="132" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B132" s="63" t="s">
+    <row r="133" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B133" s="62" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="133" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B133" s="63" t="s">
+    <row r="134" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B134" s="62" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="134" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B134" s="63" t="s">
+    <row r="135" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B135" s="62" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="135" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B135" s="63" t="s">
+    <row r="136" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B136" s="62" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="136" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B136" s="63" t="s">
+    <row r="137" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B137" s="62" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="137" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B137" s="63" t="s">
+    <row r="138" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B138" s="62" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="138" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B138" s="63" t="s">
+    <row r="139" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B139" s="62" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="139" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B139" s="63" t="s">
+    <row r="140" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B140" s="62" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="140" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B140" s="63" t="s">
+    <row r="141" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B141" s="62" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="141" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B141" s="63" t="s">
+    <row r="142" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B142" s="62" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="142" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B142" s="63" t="s">
+    <row r="143" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B143" s="62" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="143" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B143" s="63" t="s">
+    <row r="144" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B144" s="62" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="144" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B144" s="63" t="s">
+    <row r="145" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B145" s="62" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="145" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B145" s="63" t="s">
+    <row r="146" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B146" s="62" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="146" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B146" s="63" t="s">
+    <row r="147" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B147" s="62" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="147" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B147" s="63" t="s">
+    <row r="148" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B148" s="62" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="148" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B148" s="63" t="s">
+    <row r="149" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B149" s="62" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="149" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B149" s="63" t="s">
+    <row r="150" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B150" s="62" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="150" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B150" s="63" t="s">
+    <row r="151" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B151" s="62" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="151" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B151" s="63" t="s">
+    <row r="152" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B152" s="62" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="152" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B152" s="63" t="s">
+    <row r="153" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B153" s="62" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="153" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B153" s="63" t="s">
+    <row r="154" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B154" s="62" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="154" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B154" s="63" t="s">
+    <row r="155" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B155" s="62" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="155" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B155" s="63" t="s">
+    <row r="156" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B156" s="62" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="156" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B156" s="63" t="s">
+    <row r="157" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B157" s="62" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="157" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B157" s="63" t="s">
+    <row r="158" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B158" s="62" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="158" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B158" s="63" t="s">
+    <row r="159" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B159" s="62" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="159" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B159" s="63" t="s">
+    <row r="160" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B160" s="62" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="160" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B160" s="63" t="s">
+    <row r="161" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B161" s="62" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="161" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B161" s="63" t="s">
+    <row r="162" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B162" s="62" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="162" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B162" s="63" t="s">
+    <row r="163" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B163" s="62" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="163" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B163" s="63" t="s">
+    <row r="164" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B164" s="62" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="164" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B164" s="63" t="s">
+    <row r="165" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B165" s="62" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="165" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B165" s="63" t="s">
+    <row r="166" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B166" s="62" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="166" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B166" s="63" t="s">
+    <row r="167" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B167" s="62" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="167" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B167" s="63" t="s">
+    <row r="168" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B168" s="62" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="168" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B168" s="63" t="s">
+    <row r="169" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B169" s="62" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="169" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B169" s="63" t="s">
+    <row r="170" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B170" s="62" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="170" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B170" s="63" t="s">
+    <row r="171" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B171" s="62" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="171" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B171" s="63" t="s">
+    <row r="172" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B172" s="62" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="172" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B172" s="63" t="s">
+    <row r="173" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B173" s="62" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="173" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B173" s="63" t="s">
+    <row r="174" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B174" s="62" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="174" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B174" s="63" t="s">
+    <row r="175" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B175" s="62" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="175" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B175" s="63" t="s">
+    <row r="176" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B176" s="62" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="176" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B176" s="63" t="s">
+    <row r="177" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B177" s="62" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="177" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B177" s="63" t="s">
+    <row r="178" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B178" s="62" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="178" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B178" s="63" t="s">
+    <row r="179" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B179" s="62" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="179" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B179" s="63" t="s">
+    <row r="180" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B180" s="62" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="180" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B180" s="63" t="s">
+    <row r="181" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B181" s="62" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="181" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B181" s="63" t="s">
+    <row r="182" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B182" s="62" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="182" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B182" s="63" t="s">
+    <row r="183" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B183" s="62" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="183" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B183" s="63" t="s">
+    <row r="184" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B184" s="62" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="184" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B184" s="63" t="s">
+    <row r="185" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B185" s="62" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="185" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B185" s="63" t="s">
+    <row r="186" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B186" s="62" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="186" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B186" s="63" t="s">
+    <row r="187" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B187" s="62" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="187" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B187" s="63" t="s">
+    <row r="188" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B188" s="62" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="188" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B188" s="63" t="s">
+    <row r="189" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B189" s="62" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="189" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B189" s="63" t="s">
+    <row r="190" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B190" s="62" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="190" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B190" s="63" t="s">
+    <row r="191" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B191" s="62" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="191" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B191" s="63" t="s">
+    <row r="192" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B192" s="62" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="192" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B192" s="63" t="s">
+    <row r="193" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B193" s="62" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="193" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B193" s="63" t="s">
+    <row r="194" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B194" s="62" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="194" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B194" s="63" t="s">
+    <row r="195" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B195" s="62" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="195" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B195" s="63" t="s">
+    <row r="196" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B196" s="62" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="196" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B196" s="63" t="s">
+    <row r="197" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B197" s="62" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="197" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B197" s="63" t="s">
+    <row r="198" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B198" s="62" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="198" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B198" s="63" t="s">
+    <row r="199" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B199" s="62" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="199" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B199" s="63" t="s">
+    <row r="200" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B200" s="62" t="s">
         <v>522</v>
-      </c>
-    </row>
-    <row r="200" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B200" s="63" t="s">
-        <v>523</v>
       </c>
     </row>
   </sheetData>
@@ -4895,7 +4767,7 @@
   <dimension ref="A1:Y85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5104,7 +4976,7 @@
         <v>183</v>
       </c>
       <c r="D4" s="49" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E4" s="36" t="s">
         <v>160</v>
@@ -5146,7 +5018,7 @@
         <v>181</v>
       </c>
       <c r="D5" s="49" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E5" s="36" t="s">
         <v>169</v>
@@ -5188,7 +5060,7 @@
         <v>182</v>
       </c>
       <c r="D6" s="49" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E6" s="36" t="s">
         <v>173</v>
@@ -5230,7 +5102,7 @@
         <v>184</v>
       </c>
       <c r="D7" s="49" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E7" s="36" t="s">
         <v>164</v>
@@ -5842,7 +5714,7 @@
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" ht="24.5" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -5856,50 +5728,50 @@
     </row>
     <row r="4" spans="1:3" ht="13.5" customHeight="1">
       <c r="A4" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="B4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A5" s="67" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A5" s="68" t="s">
+      <c r="B5" s="67" t="s">
         <v>553</v>
       </c>
-      <c r="B5" s="68" t="s">
+    </row>
+    <row r="6" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A6" s="67" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="67" t="s">
         <v>554</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A6" s="68" t="s">
-        <v>107</v>
-      </c>
-      <c r="B6" s="68" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="13.5" customHeight="1">
       <c r="A7" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>556</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="13.5" customHeight="1">
       <c r="A8" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>558</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="13.5" customHeight="1">
       <c r="A9" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>560</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>561</v>
       </c>
     </row>
   </sheetData>
@@ -5941,7 +5813,7 @@
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" ht="18" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -5958,23 +5830,23 @@
         <v>105</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="13.5" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="13.5" customHeight="1">
       <c r="A6" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>565</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="13.5" customHeight="1">
@@ -5987,18 +5859,18 @@
     </row>
     <row r="8" spans="1:3" ht="13.5" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="13.5" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="13.5" customHeight="1">
@@ -6006,7 +5878,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
   </sheetData>
@@ -6027,7 +5899,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6207,8 +6079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ6"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6301,8 +6173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE28"/>
   <sheetViews>
-    <sheetView topLeftCell="L2" workbookViewId="0">
-      <selection activeCell="AD4" sqref="AD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6440,11 +6312,11 @@
       <c r="M2" s="25"/>
       <c r="N2" s="25"/>
       <c r="O2" s="25"/>
-      <c r="P2" s="53" t="s">
+      <c r="P2" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="53"/>
+      <c r="Q2" s="68"/>
+      <c r="R2" s="68"/>
       <c r="Z2" s="25"/>
       <c r="AC2" s="26"/>
       <c r="AD2" s="26"/>
@@ -6553,10 +6425,10 @@
         <v>209</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F4" s="15" t="s">
         <v>109</v>
@@ -6626,7 +6498,7 @@
     </row>
     <row r="5" spans="1:31" ht="13.5" customHeight="1">
       <c r="A5" s="19" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>210</v>
@@ -6638,7 +6510,7 @@
         <v>210</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F5" s="15" t="s">
         <v>109</v>
@@ -6715,7 +6587,7 @@
         <v>213</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>90</v>
@@ -7119,13 +6991,13 @@
         <v>226</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>227</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>90</v>
@@ -7453,7 +7325,7 @@
         <v>238</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>90</v>
@@ -7535,7 +7407,7 @@
         <v>239</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>90</v>
@@ -7617,7 +7489,7 @@
         <v>242</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>90</v>
@@ -8017,19 +7889,19 @@
       <c r="AD21" s="33"/>
     </row>
     <row r="22" spans="1:31">
-      <c r="A22" s="54" t="s">
+      <c r="A22" s="53" t="s">
         <v>255</v>
       </c>
-      <c r="B22" s="54" t="s">
+      <c r="B22" s="53" t="s">
         <v>254</v>
       </c>
-      <c r="C22" s="55" t="s">
-        <v>256</v>
-      </c>
-      <c r="D22" s="56" t="s">
+      <c r="C22" s="54" t="s">
+        <v>569</v>
+      </c>
+      <c r="D22" s="55" t="s">
         <v>254</v>
       </c>
-      <c r="E22" s="56" t="s">
+      <c r="E22" s="55" t="s">
         <v>90</v>
       </c>
       <c r="F22" s="15" t="s">
@@ -8038,81 +7910,81 @@
       <c r="G22" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="H22" s="57">
-        <v>0</v>
-      </c>
-      <c r="I22" s="56" t="s">
+      <c r="H22" s="56">
+        <v>0</v>
+      </c>
+      <c r="I22" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="J22" s="58" t="s">
+      <c r="J22" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="K22" s="54">
+      <c r="K22" s="53">
         <v>2</v>
       </c>
-      <c r="L22" s="59">
+      <c r="L22" s="58">
         <v>7</v>
       </c>
-      <c r="M22" s="59">
-        <v>0</v>
-      </c>
-      <c r="N22" s="59">
+      <c r="M22" s="58">
+        <v>0</v>
+      </c>
+      <c r="N22" s="58">
         <v>1000000000</v>
       </c>
-      <c r="O22" s="59">
-        <v>0</v>
-      </c>
-      <c r="P22" s="60">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="60">
+      <c r="O22" s="58">
+        <v>0</v>
+      </c>
+      <c r="P22" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="59">
         <v>2</v>
       </c>
-      <c r="R22" s="60">
-        <v>0</v>
-      </c>
-      <c r="S22" s="54">
+      <c r="R22" s="59">
+        <v>0</v>
+      </c>
+      <c r="S22" s="53">
         <v>10</v>
       </c>
-      <c r="T22" s="54">
+      <c r="T22" s="53">
         <v>7.5</v>
       </c>
-      <c r="U22" s="54">
+      <c r="U22" s="53">
         <v>14</v>
       </c>
-      <c r="V22" s="54">
+      <c r="V22" s="53">
         <v>1</v>
       </c>
-      <c r="W22" s="56"/>
-      <c r="X22" s="61"/>
-      <c r="Y22" s="61"/>
-      <c r="Z22" s="59">
+      <c r="W22" s="55"/>
+      <c r="X22" s="60"/>
+      <c r="Y22" s="60"/>
+      <c r="Z22" s="58">
         <v>10</v>
       </c>
-      <c r="AA22" s="60">
-        <v>0</v>
-      </c>
-      <c r="AB22" s="60">
-        <v>0</v>
-      </c>
-      <c r="AC22" s="61"/>
-      <c r="AD22" s="61"/>
-      <c r="AE22" s="55"/>
+      <c r="AA22" s="59">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="59">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="60"/>
+      <c r="AD22" s="60"/>
+      <c r="AE22" s="54"/>
     </row>
     <row r="23" spans="1:31">
-      <c r="A23" s="54" t="s">
+      <c r="A23" s="53" t="s">
+        <v>256</v>
+      </c>
+      <c r="B23" s="53" t="s">
         <v>257</v>
       </c>
-      <c r="B23" s="54" t="s">
+      <c r="C23" s="54" t="s">
         <v>258</v>
       </c>
-      <c r="C23" s="55" t="s">
-        <v>259</v>
-      </c>
-      <c r="D23" s="56" t="s">
-        <v>258</v>
-      </c>
-      <c r="E23" s="56" t="s">
+      <c r="D23" s="55" t="s">
+        <v>257</v>
+      </c>
+      <c r="E23" s="55" t="s">
         <v>90</v>
       </c>
       <c r="F23" s="15" t="s">
@@ -8121,81 +7993,81 @@
       <c r="G23" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="H23" s="57">
-        <v>0</v>
-      </c>
-      <c r="I23" s="56" t="s">
+      <c r="H23" s="56">
+        <v>0</v>
+      </c>
+      <c r="I23" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="J23" s="58" t="s">
+      <c r="J23" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="K23" s="54">
+      <c r="K23" s="53">
         <v>2</v>
       </c>
-      <c r="L23" s="59">
+      <c r="L23" s="58">
         <v>7</v>
       </c>
-      <c r="M23" s="59">
-        <v>0</v>
-      </c>
-      <c r="N23" s="59">
+      <c r="M23" s="58">
+        <v>0</v>
+      </c>
+      <c r="N23" s="58">
         <v>1000000000</v>
       </c>
-      <c r="O23" s="59">
-        <v>0</v>
-      </c>
-      <c r="P23" s="60">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="60">
+      <c r="O23" s="58">
+        <v>0</v>
+      </c>
+      <c r="P23" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="59">
         <v>2</v>
       </c>
-      <c r="R23" s="60">
-        <v>0</v>
-      </c>
-      <c r="S23" s="54">
+      <c r="R23" s="59">
+        <v>0</v>
+      </c>
+      <c r="S23" s="53">
         <v>10</v>
       </c>
-      <c r="T23" s="54">
+      <c r="T23" s="53">
         <v>7.5</v>
       </c>
-      <c r="U23" s="54">
+      <c r="U23" s="53">
         <v>14</v>
       </c>
-      <c r="V23" s="54">
+      <c r="V23" s="53">
         <v>1</v>
       </c>
-      <c r="W23" s="56"/>
-      <c r="X23" s="61"/>
-      <c r="Y23" s="61"/>
-      <c r="Z23" s="59">
+      <c r="W23" s="55"/>
+      <c r="X23" s="60"/>
+      <c r="Y23" s="60"/>
+      <c r="Z23" s="58">
         <v>10</v>
       </c>
-      <c r="AA23" s="60">
-        <v>0</v>
-      </c>
-      <c r="AB23" s="60">
-        <v>0</v>
-      </c>
-      <c r="AC23" s="61"/>
-      <c r="AD23" s="61"/>
-      <c r="AE23" s="55"/>
+      <c r="AA23" s="59">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="59">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="60"/>
+      <c r="AD23" s="60"/>
+      <c r="AE23" s="54"/>
     </row>
     <row r="24" spans="1:31">
-      <c r="A24" s="54" t="s">
-        <v>261</v>
-      </c>
-      <c r="B24" s="54" t="s">
-        <v>261</v>
-      </c>
-      <c r="C24" s="55" t="s">
+      <c r="A24" s="53" t="s">
         <v>260</v>
       </c>
-      <c r="D24" s="56" t="s">
-        <v>544</v>
-      </c>
-      <c r="E24" s="56" t="s">
+      <c r="B24" s="53" t="s">
+        <v>260</v>
+      </c>
+      <c r="C24" s="54" t="s">
+        <v>259</v>
+      </c>
+      <c r="D24" s="55" t="s">
+        <v>543</v>
+      </c>
+      <c r="E24" s="55" t="s">
         <v>90</v>
       </c>
       <c r="F24" s="15" t="s">
@@ -8204,81 +8076,81 @@
       <c r="G24" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="H24" s="57">
-        <v>0</v>
-      </c>
-      <c r="I24" s="56" t="s">
+      <c r="H24" s="56">
+        <v>0</v>
+      </c>
+      <c r="I24" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="J24" s="58" t="s">
+      <c r="J24" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="K24" s="54">
+      <c r="K24" s="53">
         <v>2</v>
       </c>
-      <c r="L24" s="59">
+      <c r="L24" s="58">
         <v>7</v>
       </c>
-      <c r="M24" s="59">
-        <v>0</v>
-      </c>
-      <c r="N24" s="59">
+      <c r="M24" s="58">
+        <v>0</v>
+      </c>
+      <c r="N24" s="58">
         <v>1000000000</v>
       </c>
-      <c r="O24" s="59">
-        <v>0</v>
-      </c>
-      <c r="P24" s="60">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="60">
+      <c r="O24" s="58">
+        <v>0</v>
+      </c>
+      <c r="P24" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="59">
         <v>2</v>
       </c>
-      <c r="R24" s="60">
-        <v>0</v>
-      </c>
-      <c r="S24" s="54">
+      <c r="R24" s="59">
+        <v>0</v>
+      </c>
+      <c r="S24" s="53">
         <v>10</v>
       </c>
-      <c r="T24" s="54">
+      <c r="T24" s="53">
         <v>7.5</v>
       </c>
-      <c r="U24" s="54">
+      <c r="U24" s="53">
         <v>14</v>
       </c>
-      <c r="V24" s="54">
+      <c r="V24" s="53">
         <v>1</v>
       </c>
-      <c r="W24" s="56"/>
-      <c r="X24" s="61"/>
-      <c r="Y24" s="61"/>
-      <c r="Z24" s="59">
+      <c r="W24" s="55"/>
+      <c r="X24" s="60"/>
+      <c r="Y24" s="60"/>
+      <c r="Z24" s="58">
         <v>10</v>
       </c>
-      <c r="AA24" s="60">
-        <v>0</v>
-      </c>
-      <c r="AB24" s="60">
-        <v>0</v>
-      </c>
-      <c r="AC24" s="61"/>
-      <c r="AD24" s="61"/>
-      <c r="AE24" s="55"/>
+      <c r="AA24" s="59">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="59">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="60"/>
+      <c r="AD24" s="60"/>
+      <c r="AE24" s="54"/>
     </row>
     <row r="25" spans="1:31">
-      <c r="A25" s="54" t="s">
+      <c r="A25" s="53" t="s">
+        <v>261</v>
+      </c>
+      <c r="B25" s="53" t="s">
         <v>262</v>
       </c>
-      <c r="B25" s="54" t="s">
+      <c r="C25" s="54" t="s">
         <v>263</v>
       </c>
-      <c r="C25" s="55" t="s">
-        <v>264</v>
-      </c>
-      <c r="D25" s="56" t="s">
-        <v>263</v>
-      </c>
-      <c r="E25" s="56" t="s">
+      <c r="D25" s="55" t="s">
+        <v>262</v>
+      </c>
+      <c r="E25" s="55" t="s">
         <v>90</v>
       </c>
       <c r="F25" s="15" t="s">
@@ -8287,81 +8159,81 @@
       <c r="G25" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="H25" s="57">
-        <v>0</v>
-      </c>
-      <c r="I25" s="56" t="s">
+      <c r="H25" s="56">
+        <v>0</v>
+      </c>
+      <c r="I25" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="J25" s="58" t="s">
+      <c r="J25" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="K25" s="54">
+      <c r="K25" s="53">
         <v>2</v>
       </c>
-      <c r="L25" s="59">
+      <c r="L25" s="58">
         <v>7</v>
       </c>
-      <c r="M25" s="59">
-        <v>0</v>
-      </c>
-      <c r="N25" s="59">
+      <c r="M25" s="58">
+        <v>0</v>
+      </c>
+      <c r="N25" s="58">
         <v>1000000000</v>
       </c>
-      <c r="O25" s="59">
-        <v>0</v>
-      </c>
-      <c r="P25" s="60">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="60">
+      <c r="O25" s="58">
+        <v>0</v>
+      </c>
+      <c r="P25" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="59">
         <v>2</v>
       </c>
-      <c r="R25" s="60">
-        <v>0</v>
-      </c>
-      <c r="S25" s="54">
+      <c r="R25" s="59">
+        <v>0</v>
+      </c>
+      <c r="S25" s="53">
         <v>10</v>
       </c>
-      <c r="T25" s="54">
+      <c r="T25" s="53">
         <v>7.5</v>
       </c>
-      <c r="U25" s="54">
+      <c r="U25" s="53">
         <v>14</v>
       </c>
-      <c r="V25" s="54">
+      <c r="V25" s="53">
         <v>1</v>
       </c>
-      <c r="W25" s="56"/>
-      <c r="X25" s="61"/>
-      <c r="Y25" s="61"/>
-      <c r="Z25" s="59">
+      <c r="W25" s="55"/>
+      <c r="X25" s="60"/>
+      <c r="Y25" s="60"/>
+      <c r="Z25" s="58">
         <v>10</v>
       </c>
-      <c r="AA25" s="60">
-        <v>0</v>
-      </c>
-      <c r="AB25" s="60">
-        <v>0</v>
-      </c>
-      <c r="AC25" s="61"/>
-      <c r="AD25" s="61"/>
-      <c r="AE25" s="55"/>
+      <c r="AA25" s="59">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="59">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="60"/>
+      <c r="AD25" s="60"/>
+      <c r="AE25" s="54"/>
     </row>
     <row r="26" spans="1:31">
-      <c r="A26" s="54" t="s">
+      <c r="A26" s="53" t="s">
+        <v>264</v>
+      </c>
+      <c r="B26" s="53" t="s">
+        <v>264</v>
+      </c>
+      <c r="C26" s="54" t="s">
         <v>265</v>
       </c>
-      <c r="B26" s="54" t="s">
-        <v>265</v>
-      </c>
-      <c r="C26" s="55" t="s">
-        <v>266</v>
-      </c>
-      <c r="D26" s="56" t="s">
-        <v>545</v>
-      </c>
-      <c r="E26" s="56" t="s">
+      <c r="D26" s="55" t="s">
+        <v>544</v>
+      </c>
+      <c r="E26" s="55" t="s">
         <v>90</v>
       </c>
       <c r="F26" s="15" t="s">
@@ -8370,81 +8242,81 @@
       <c r="G26" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="H26" s="57">
-        <v>0</v>
-      </c>
-      <c r="I26" s="56" t="s">
+      <c r="H26" s="56">
+        <v>0</v>
+      </c>
+      <c r="I26" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="J26" s="58" t="s">
+      <c r="J26" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="K26" s="54">
+      <c r="K26" s="53">
         <v>2</v>
       </c>
-      <c r="L26" s="59">
+      <c r="L26" s="58">
         <v>7</v>
       </c>
-      <c r="M26" s="59">
-        <v>0</v>
-      </c>
-      <c r="N26" s="59">
+      <c r="M26" s="58">
+        <v>0</v>
+      </c>
+      <c r="N26" s="58">
         <v>1000000000</v>
       </c>
-      <c r="O26" s="59">
-        <v>0</v>
-      </c>
-      <c r="P26" s="60">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="60">
+      <c r="O26" s="58">
+        <v>0</v>
+      </c>
+      <c r="P26" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="59">
         <v>2</v>
       </c>
-      <c r="R26" s="60">
-        <v>0</v>
-      </c>
-      <c r="S26" s="54">
+      <c r="R26" s="59">
+        <v>0</v>
+      </c>
+      <c r="S26" s="53">
         <v>10</v>
       </c>
-      <c r="T26" s="54">
+      <c r="T26" s="53">
         <v>7.5</v>
       </c>
-      <c r="U26" s="54">
+      <c r="U26" s="53">
         <v>14</v>
       </c>
-      <c r="V26" s="54">
+      <c r="V26" s="53">
         <v>1</v>
       </c>
-      <c r="W26" s="56"/>
-      <c r="X26" s="61"/>
-      <c r="Y26" s="61"/>
-      <c r="Z26" s="59">
+      <c r="W26" s="55"/>
+      <c r="X26" s="60"/>
+      <c r="Y26" s="60"/>
+      <c r="Z26" s="58">
         <v>10</v>
       </c>
-      <c r="AA26" s="60">
-        <v>0</v>
-      </c>
-      <c r="AB26" s="60">
-        <v>0</v>
-      </c>
-      <c r="AC26" s="61"/>
-      <c r="AD26" s="61"/>
-      <c r="AE26" s="55"/>
+      <c r="AA26" s="59">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="59">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="60"/>
+      <c r="AD26" s="60"/>
+      <c r="AE26" s="54"/>
     </row>
     <row r="27" spans="1:31">
-      <c r="A27" s="54" t="s">
+      <c r="A27" s="53" t="s">
+        <v>266</v>
+      </c>
+      <c r="B27" s="53" t="s">
         <v>267</v>
       </c>
-      <c r="B27" s="54" t="s">
+      <c r="C27" s="54" t="s">
         <v>268</v>
       </c>
-      <c r="C27" s="55" t="s">
-        <v>269</v>
-      </c>
-      <c r="D27" s="56" t="s">
-        <v>268</v>
-      </c>
-      <c r="E27" s="56" t="s">
+      <c r="D27" s="55" t="s">
+        <v>267</v>
+      </c>
+      <c r="E27" s="55" t="s">
         <v>90</v>
       </c>
       <c r="F27" s="15" t="s">
@@ -8453,81 +8325,81 @@
       <c r="G27" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="H27" s="57">
-        <v>0</v>
-      </c>
-      <c r="I27" s="56" t="s">
+      <c r="H27" s="56">
+        <v>0</v>
+      </c>
+      <c r="I27" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="J27" s="58" t="s">
+      <c r="J27" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="K27" s="54">
+      <c r="K27" s="53">
         <v>2</v>
       </c>
-      <c r="L27" s="59">
+      <c r="L27" s="58">
         <v>7</v>
       </c>
-      <c r="M27" s="59">
-        <v>0</v>
-      </c>
-      <c r="N27" s="59">
+      <c r="M27" s="58">
+        <v>0</v>
+      </c>
+      <c r="N27" s="58">
         <v>1000000000</v>
       </c>
-      <c r="O27" s="59">
-        <v>0</v>
-      </c>
-      <c r="P27" s="60">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="60">
+      <c r="O27" s="58">
+        <v>0</v>
+      </c>
+      <c r="P27" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="59">
         <v>2</v>
       </c>
-      <c r="R27" s="60">
-        <v>0</v>
-      </c>
-      <c r="S27" s="54">
+      <c r="R27" s="59">
+        <v>0</v>
+      </c>
+      <c r="S27" s="53">
         <v>10</v>
       </c>
-      <c r="T27" s="54">
+      <c r="T27" s="53">
         <v>7.5</v>
       </c>
-      <c r="U27" s="54">
+      <c r="U27" s="53">
         <v>14</v>
       </c>
-      <c r="V27" s="54">
+      <c r="V27" s="53">
         <v>1</v>
       </c>
-      <c r="W27" s="56"/>
-      <c r="X27" s="61"/>
-      <c r="Y27" s="61"/>
-      <c r="Z27" s="59">
+      <c r="W27" s="55"/>
+      <c r="X27" s="60"/>
+      <c r="Y27" s="60"/>
+      <c r="Z27" s="58">
         <v>10</v>
       </c>
-      <c r="AA27" s="60">
-        <v>0</v>
-      </c>
-      <c r="AB27" s="60">
-        <v>0</v>
-      </c>
-      <c r="AC27" s="61"/>
-      <c r="AD27" s="61"/>
-      <c r="AE27" s="55"/>
+      <c r="AA27" s="59">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="59">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="60"/>
+      <c r="AD27" s="60"/>
+      <c r="AE27" s="54"/>
     </row>
     <row r="28" spans="1:31">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="53" t="s">
+        <v>270</v>
+      </c>
+      <c r="B28" s="53" t="s">
+        <v>269</v>
+      </c>
+      <c r="C28" s="54" t="s">
         <v>271</v>
       </c>
-      <c r="B28" s="54" t="s">
-        <v>270</v>
-      </c>
-      <c r="C28" s="55" t="s">
-        <v>272</v>
-      </c>
-      <c r="D28" s="56" t="s">
-        <v>270</v>
-      </c>
-      <c r="E28" s="56" t="s">
+      <c r="D28" s="55" t="s">
+        <v>269</v>
+      </c>
+      <c r="E28" s="55" t="s">
         <v>90</v>
       </c>
       <c r="F28" s="15" t="s">
@@ -8536,66 +8408,66 @@
       <c r="G28" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="H28" s="57">
-        <v>0</v>
-      </c>
-      <c r="I28" s="56" t="s">
+      <c r="H28" s="56">
+        <v>0</v>
+      </c>
+      <c r="I28" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="J28" s="58" t="s">
+      <c r="J28" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="K28" s="54">
+      <c r="K28" s="53">
         <v>2</v>
       </c>
-      <c r="L28" s="59">
+      <c r="L28" s="58">
         <v>7</v>
       </c>
-      <c r="M28" s="59">
-        <v>0</v>
-      </c>
-      <c r="N28" s="59">
+      <c r="M28" s="58">
+        <v>0</v>
+      </c>
+      <c r="N28" s="58">
         <v>1000000000</v>
       </c>
-      <c r="O28" s="59">
-        <v>0</v>
-      </c>
-      <c r="P28" s="60">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="60">
+      <c r="O28" s="58">
+        <v>0</v>
+      </c>
+      <c r="P28" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="59">
         <v>2</v>
       </c>
-      <c r="R28" s="60">
-        <v>0</v>
-      </c>
-      <c r="S28" s="54">
+      <c r="R28" s="59">
+        <v>0</v>
+      </c>
+      <c r="S28" s="53">
         <v>10</v>
       </c>
-      <c r="T28" s="54">
+      <c r="T28" s="53">
         <v>7.5</v>
       </c>
-      <c r="U28" s="54">
+      <c r="U28" s="53">
         <v>14</v>
       </c>
-      <c r="V28" s="54">
+      <c r="V28" s="53">
         <v>1</v>
       </c>
-      <c r="W28" s="56"/>
-      <c r="X28" s="61"/>
-      <c r="Y28" s="61"/>
-      <c r="Z28" s="59">
+      <c r="W28" s="55"/>
+      <c r="X28" s="60"/>
+      <c r="Y28" s="60"/>
+      <c r="Z28" s="58">
         <v>10</v>
       </c>
-      <c r="AA28" s="60">
-        <v>0</v>
-      </c>
-      <c r="AB28" s="60">
-        <v>0</v>
-      </c>
-      <c r="AC28" s="61"/>
-      <c r="AD28" s="61"/>
-      <c r="AE28" s="55"/>
+      <c r="AA28" s="59">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="59">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="60"/>
+      <c r="AD28" s="60"/>
+      <c r="AE28" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8620,7 +8492,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="167" yWindow="253" count="13">
@@ -8714,15 +8585,6 @@
           </x14:formula2>
           <xm:sqref>H4:H21</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" operator="equal" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Select a valid entry from the drop-down menu" promptTitle="Field or Lab analysis?" prompt="Select a valid entry from the drop-down menu">
-          <x14:formula1>
-            <xm:f>[1]Constants!#REF!</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>E4:E21</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Select a valid entry from the drop-down menu" promptTitle="Valid categories" prompt="Select a valid entry from the drop-down menu">
           <x14:formula1>
             <xm:f>'Analysis Categories'!$A$4:$A$44</xm:f>
@@ -8734,6 +8596,12 @@
             <xm:f>'Lab Departments'!$A$4:$A$49</xm:f>
           </x14:formula1>
           <xm:sqref>G4:G28</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" operator="equal" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Select a valid entry from the drop-down menu" promptTitle="Field or Lab analysis?" prompt="Select a valid entry from the drop-down menu">
+          <x14:formula1>
+            <xm:f>Constants!$K$2:$K$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>E4:E28</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -8813,7 +8681,7 @@
     <row r="4" spans="1:15" ht="13.5" customHeight="1">
       <c r="A4" s="14"/>
       <c r="B4" s="17" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>198</v>
@@ -8843,7 +8711,7 @@
         <v>203</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="13.5" customHeight="1">
@@ -8897,7 +8765,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8933,7 +8801,7 @@
     </row>
     <row r="4" spans="1:3" s="12" customFormat="1" ht="12.25" customHeight="1">
       <c r="A4" s="14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>224</v>
@@ -8941,7 +8809,7 @@
     </row>
     <row r="5" spans="1:3" ht="13.5" customHeight="1">
       <c r="A5" s="14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>218</v>
@@ -8949,7 +8817,7 @@
     </row>
     <row r="6" spans="1:3" ht="13.5" customHeight="1">
       <c r="A6" s="14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>215</v>
@@ -8957,7 +8825,7 @@
     </row>
     <row r="7" spans="1:3" ht="13.5" customHeight="1">
       <c r="A7" s="14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>237</v>
@@ -8965,7 +8833,7 @@
     </row>
     <row r="8" spans="1:3" ht="13.5" customHeight="1">
       <c r="A8" s="14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>226</v>
@@ -8973,7 +8841,7 @@
     </row>
     <row r="9" spans="1:3" ht="13.5" customHeight="1">
       <c r="A9" s="14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>231</v>
@@ -8981,7 +8849,7 @@
     </row>
     <row r="10" spans="1:3" ht="13.5" customHeight="1">
       <c r="A10" s="14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>221</v>
@@ -8989,7 +8857,7 @@
     </row>
     <row r="11" spans="1:3" ht="13.5" customHeight="1">
       <c r="A11" s="14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>212</v>
@@ -8997,7 +8865,7 @@
     </row>
     <row r="12" spans="1:3" ht="13.5" customHeight="1">
       <c r="A12" s="14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>218</v>
@@ -9005,7 +8873,7 @@
     </row>
     <row r="13" spans="1:3" ht="13.5" customHeight="1">
       <c r="A13" s="14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>234</v>
@@ -9013,15 +8881,15 @@
     </row>
     <row r="14" spans="1:3" ht="13.5" customHeight="1">
       <c r="A14" s="14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="13.5" customHeight="1">
       <c r="A15" s="14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>207</v>
@@ -9048,7 +8916,7 @@
         <v>204</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="13.5" customHeight="1">
@@ -9056,7 +8924,7 @@
         <v>204</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="13.5" customHeight="1">
@@ -9064,7 +8932,7 @@
         <v>204</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="13.5" customHeight="1">
@@ -9072,7 +8940,7 @@
         <v>204</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="13.5" customHeight="1">
@@ -9080,7 +8948,7 @@
         <v>204</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -9104,7 +8972,7 @@
         <v>202</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -9128,7 +8996,6 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">

</xml_diff>

<commit_message>
INFRA-249: Pull results from SENAITE and save them to OpenMRS and Bahmni
</commit_message>
<xml_diff>
--- a/configuration/senaite/configuration.xlsx
+++ b/configuration/senaite/configuration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="0" windowWidth="25040" windowHeight="16600" tabRatio="950" firstSheet="2" activeTab="10"/>
+    <workbookView xWindow="600" yWindow="0" windowWidth="27520" windowHeight="15500" tabRatio="950" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Lab Departments" sheetId="12" r:id="rId1"/>
@@ -22,7 +22,6 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId13"/>
-    <externalReference r:id="rId14"/>
   </externalReferences>
   <calcPr calcId="140000" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -827,9 +826,6 @@
     <t>VERY LOW DENSITY LIPOPROTEIN</t>
   </si>
   <si>
-    <t>Very Low Density Lipoprotein (VLDL) is one of three major lipoprotein particles.  VLDL contains the highest amount of triglyceride. Since VLDL contains most of the circulating triglyceride and since the compositions of the different particles are relatively constant, it is possible to estimate the amount of VLDL cholesterol by dividing the triglyceride value (in mg/dL) by 5 (1298AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA)</t>
-  </si>
-  <si>
     <t>HIGH-DENSITY LIPOPROTEIN CHOLESTEROL</t>
   </si>
   <si>
@@ -1767,6 +1763,9 @@
   </si>
   <si>
     <t>Different type water samples</t>
+  </si>
+  <si>
+    <t>Very Low Density Lipoprotein {VLDL} is one of three major lipoprotein particles.  VLDL contains the highest amount of triglyceride. Since VLDL contains most of the circulating triglyceride and since the compositions of the different particles are relatively constant, it is possible to estimate the amount of VLDL cholesterol by dividing the triglyceride value (in mg/dL) by 5 (1298AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA)</t>
   </si>
 </sst>
 </file>
@@ -1958,7 +1957,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1978,6 +1977,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2146,9 +2148,6 @@
     <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -2190,8 +2189,11 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="44">
+  <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2225,6 +2227,9 @@
     <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2368,137 +2373,6 @@
       <sheetData sheetId="57"/>
       <sheetData sheetId="58"/>
       <sheetData sheetId="59"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Instructions"/>
-      <sheetName val="Lab Information"/>
-      <sheetName val="Lab Contacts"/>
-      <sheetName val="Lab Departments"/>
-      <sheetName val="Lab Products"/>
-      <sheetName val="Clients"/>
-      <sheetName val="Client Contacts"/>
-      <sheetName val="Attachment Types"/>
-      <sheetName val="Container Types"/>
-      <sheetName val="Preservations"/>
-      <sheetName val="Storage Locations"/>
-      <sheetName val="Supply Orders"/>
-      <sheetName val="Containers"/>
-      <sheetName val="Sample Matrices"/>
-      <sheetName val="Sample Types"/>
-      <sheetName val="Sample Points"/>
-      <sheetName val="Sample Point Sample Types"/>
-      <sheetName val="Methods"/>
-      <sheetName val="Manufacturers"/>
-      <sheetName val="Suppliers"/>
-      <sheetName val="Supplier Contacts"/>
-      <sheetName val="Instrument Types"/>
-      <sheetName val="Instruments"/>
-      <sheetName val="Instrument Validations"/>
-      <sheetName val="Instrument Calibrations"/>
-      <sheetName val="Instrument Documents"/>
-      <sheetName val="Instrument Certifications"/>
-      <sheetName val="Instrument Maintenance Tasks"/>
-      <sheetName val="Instrument Schedule"/>
-      <sheetName val="Analysis Categories"/>
-      <sheetName val="Calculations"/>
-      <sheetName val="Calculation Interim Fields"/>
-      <sheetName val="Analysis Services"/>
-      <sheetName val="AnalysisService Methods"/>
-      <sheetName val="AnalysisService Instruments"/>
-      <sheetName val="AnalysisService InterimFields"/>
-      <sheetName val="AnalysisService ResultOptions"/>
-      <sheetName val="Analysis Service Uncertainties"/>
-      <sheetName val="Analysis Profiles"/>
-      <sheetName val="Analysis Profile Services"/>
-      <sheetName val="Analysis Specifications"/>
-      <sheetName val="AR Templates"/>
-      <sheetName val="AR Template Analyses"/>
-      <sheetName val="AR Template Partitions"/>
-      <sheetName val="Reference Definitions"/>
-      <sheetName val="Reference Definition Results"/>
-      <sheetName val="Reference Samples"/>
-      <sheetName val="Reference Sample Results"/>
-      <sheetName val="Reference Analyses"/>
-      <sheetName val="Reference Analyses Interims"/>
-      <sheetName val="Sample Conditions"/>
-      <sheetName val="Sampling Deviations"/>
-      <sheetName val="Analysis Requests"/>
-      <sheetName val="Analyses"/>
-      <sheetName val="Analysis Interims"/>
-      <sheetName val="Worksheet Templates"/>
-      <sheetName val="Worksheet Template Services"/>
-      <sheetName val="Worksheet Template Layouts"/>
-      <sheetName val="Setup"/>
-      <sheetName val="Constants"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
-      <sheetData sheetId="34" refreshError="1"/>
-      <sheetData sheetId="35" refreshError="1"/>
-      <sheetData sheetId="36" refreshError="1"/>
-      <sheetData sheetId="37" refreshError="1"/>
-      <sheetData sheetId="38" refreshError="1"/>
-      <sheetData sheetId="39" refreshError="1"/>
-      <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41" refreshError="1"/>
-      <sheetData sheetId="42" refreshError="1"/>
-      <sheetData sheetId="43" refreshError="1"/>
-      <sheetData sheetId="44" refreshError="1"/>
-      <sheetData sheetId="45" refreshError="1"/>
-      <sheetData sheetId="46" refreshError="1"/>
-      <sheetData sheetId="47" refreshError="1"/>
-      <sheetData sheetId="48" refreshError="1"/>
-      <sheetData sheetId="49" refreshError="1"/>
-      <sheetData sheetId="50" refreshError="1"/>
-      <sheetData sheetId="51" refreshError="1"/>
-      <sheetData sheetId="52" refreshError="1"/>
-      <sheetData sheetId="53" refreshError="1"/>
-      <sheetData sheetId="54" refreshError="1"/>
-      <sheetData sheetId="55" refreshError="1"/>
-      <sheetData sheetId="56" refreshError="1"/>
-      <sheetData sheetId="57" refreshError="1"/>
-      <sheetData sheetId="58" refreshError="1"/>
-      <sheetData sheetId="59" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2999,7 +2873,7 @@
   <dimension ref="A1:AMJ9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3082,18 +2956,18 @@
     </row>
     <row r="4" spans="1:1024" ht="13.5" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="9" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>189</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="H4" s="10">
         <v>0</v>
@@ -3101,11 +2975,11 @@
     </row>
     <row r="5" spans="1:1024" ht="13.5" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="9" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>189</v>
@@ -3120,11 +2994,11 @@
     </row>
     <row r="6" spans="1:1024">
       <c r="A6" s="9" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>189</v>
@@ -3139,11 +3013,11 @@
     </row>
     <row r="7" spans="1:1024">
       <c r="A7" s="9" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="9" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>189</v>
@@ -3158,11 +3032,11 @@
     </row>
     <row r="8" spans="1:1024">
       <c r="A8" s="19" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>189</v>
@@ -3174,11 +3048,11 @@
     </row>
     <row r="9" spans="1:1024">
       <c r="A9" s="19" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="9" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>189</v>
@@ -3193,7 +3067,6 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
@@ -3255,8 +3128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3298,219 +3171,219 @@
     </row>
     <row r="4" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="C4" s="67" t="s">
+      <c r="C4" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="C5" s="67" t="s">
+      <c r="C5" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="C6" s="67" t="s">
+      <c r="C6" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="C7" s="67" t="s">
+      <c r="C7" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="C8" s="67" t="s">
+      <c r="C8" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="C9" s="67" t="s">
+      <c r="C9" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="C10" s="67" t="s">
+      <c r="C10" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="C11" s="67" t="s">
+      <c r="C11" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="C12" s="67" t="s">
+      <c r="C12" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="C13" s="67" t="s">
+      <c r="C13" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A14" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>548</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>549</v>
-      </c>
-      <c r="C14" s="67" t="s">
+      <c r="C14" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="C15" s="67" t="s">
+      <c r="C15" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="C16" s="67" t="s">
+      <c r="C16" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="C17" s="67" t="s">
+      <c r="C17" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="C18" s="67" t="s">
+      <c r="C18" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A19" s="9" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="C19" s="67" t="s">
+      <c r="C19" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C20" s="67" t="s">
+        <v>256</v>
+      </c>
+      <c r="C20" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A21" s="9" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="C21" s="67" t="s">
+      <c r="C21" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="C22" s="67" t="s">
+      <c r="C22" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A23" s="9" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>24</v>
@@ -3518,51 +3391,51 @@
     </row>
     <row r="24" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>271</v>
-      </c>
-      <c r="C24" s="67" t="s">
+        <v>270</v>
+      </c>
+      <c r="C24" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A25" s="9" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="C25" s="67" t="s">
+        <v>261</v>
+      </c>
+      <c r="C25" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>265</v>
-      </c>
-      <c r="C26" s="67" t="s">
+        <v>264</v>
+      </c>
+      <c r="C26" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="6" customFormat="1" ht="12.25" customHeight="1">
       <c r="A27" s="9" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="C27" s="67" t="s">
+        <v>260</v>
+      </c>
+      <c r="C27" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="13.5" customHeight="1">
       <c r="A28" s="19" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>244</v>
@@ -3573,7 +3446,7 @@
     </row>
     <row r="29" spans="1:3" ht="13.5" customHeight="1">
       <c r="A29" s="19" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>246</v>
@@ -3587,7 +3460,6 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
@@ -3641,35 +3513,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="28" customFormat="1" ht="44.75" customHeight="1">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="61" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="61" t="s">
         <v>125</v>
       </c>
       <c r="C1" s="39" t="s">
+        <v>273</v>
+      </c>
+      <c r="D1" s="39" t="s">
         <v>274</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="E1" s="39" t="s">
         <v>275</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="F1" s="28" t="s">
         <v>276</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="G1" s="61" t="s">
         <v>277</v>
       </c>
-      <c r="G1" s="62" t="s">
+      <c r="H1" s="39" t="s">
         <v>278</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="I1" s="39" t="s">
         <v>279</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="J1" s="39" t="s">
         <v>280</v>
-      </c>
-      <c r="J1" s="39" t="s">
-        <v>281</v>
       </c>
       <c r="K1" s="39" t="s">
         <v>66</v>
@@ -3678,1202 +3550,1202 @@
     </row>
     <row r="2" spans="1:12" ht="13.5" customHeight="1">
       <c r="A2" s="43" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B2" s="43" t="s">
         <v>168</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="62" t="s">
+        <v>282</v>
+      </c>
+      <c r="D2" s="62" t="s">
         <v>283</v>
       </c>
-      <c r="D2" s="63" t="s">
+      <c r="E2" s="62" t="s">
         <v>284</v>
       </c>
-      <c r="E2" s="63" t="s">
+      <c r="F2" s="62" t="s">
         <v>285</v>
       </c>
-      <c r="F2" s="63" t="s">
+      <c r="G2" s="62">
+        <v>0</v>
+      </c>
+      <c r="H2" s="62" t="s">
         <v>286</v>
       </c>
-      <c r="G2" s="63">
-        <v>0</v>
-      </c>
-      <c r="H2" s="63" t="s">
+      <c r="I2" s="62" t="s">
         <v>287</v>
       </c>
-      <c r="I2" s="63" t="s">
+      <c r="J2" s="62" t="s">
         <v>288</v>
       </c>
-      <c r="J2" s="63" t="s">
-        <v>289</v>
-      </c>
-      <c r="K2" s="63" t="s">
+      <c r="K2" s="62" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="13.5" customHeight="1">
       <c r="A3" s="43" t="s">
+        <v>289</v>
+      </c>
+      <c r="B3" s="43" t="s">
         <v>290</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="C3" s="62" t="s">
         <v>291</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="D3" s="62" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="62" t="s">
         <v>292</v>
       </c>
-      <c r="D3" s="63" t="s">
-        <v>88</v>
-      </c>
-      <c r="E3" s="63" t="s">
+      <c r="F3" s="62" t="s">
         <v>293</v>
       </c>
-      <c r="F3" s="63" t="s">
+      <c r="G3" s="62">
+        <v>1</v>
+      </c>
+      <c r="H3" s="62" t="s">
         <v>294</v>
       </c>
-      <c r="G3" s="63">
-        <v>1</v>
-      </c>
-      <c r="H3" s="63" t="s">
+      <c r="I3" s="62" t="s">
         <v>295</v>
       </c>
-      <c r="I3" s="63" t="s">
+      <c r="J3" s="62" t="s">
         <v>296</v>
       </c>
-      <c r="J3" s="63" t="s">
-        <v>297</v>
-      </c>
-      <c r="K3" s="63" t="s">
+      <c r="K3" s="62" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="24.5" customHeight="1">
       <c r="A4" s="43" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B4" s="43" t="s">
         <v>158</v>
       </c>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="62" t="s">
+        <v>298</v>
+      </c>
+      <c r="D4" s="62" t="s">
         <v>299</v>
       </c>
-      <c r="D4" s="63" t="s">
+      <c r="F4" s="62" t="s">
         <v>300</v>
       </c>
-      <c r="F4" s="63" t="s">
+      <c r="G4" s="62"/>
+      <c r="H4" s="62" t="s">
         <v>301</v>
       </c>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63" t="s">
-        <v>302</v>
-      </c>
     </row>
     <row r="5" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="62" t="s">
         <v>179</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="62" t="s">
         <v>180</v>
       </c>
-      <c r="G5" s="63"/>
+      <c r="G5" s="62"/>
     </row>
     <row r="6" spans="1:12" ht="13.5" customHeight="1">
       <c r="A6" s="43" t="s">
+        <v>302</v>
+      </c>
+      <c r="B6" s="43" t="s">
         <v>303</v>
       </c>
-      <c r="B6" s="43" t="s">
-        <v>304</v>
-      </c>
-      <c r="G6" s="63"/>
+      <c r="G6" s="62"/>
     </row>
     <row r="7" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A7" s="63" t="s">
+      <c r="A7" s="62" t="s">
         <v>177</v>
       </c>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="62" t="s">
         <v>178</v>
       </c>
-      <c r="G7" s="63"/>
+      <c r="G7" s="62"/>
     </row>
     <row r="8" spans="1:12" ht="13.5" customHeight="1">
       <c r="A8" s="43" t="s">
+        <v>304</v>
+      </c>
+      <c r="B8" s="43" t="s">
         <v>305</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="G8" s="62"/>
+    </row>
+    <row r="9" spans="1:12" ht="13.5" customHeight="1">
+      <c r="G9" s="62"/>
+    </row>
+    <row r="10" spans="1:12" ht="13.5" customHeight="1">
+      <c r="G10" s="62"/>
+    </row>
+    <row r="11" spans="1:12" ht="13.5" customHeight="1">
+      <c r="G11" s="62"/>
+    </row>
+    <row r="12" spans="1:12" ht="13.5" customHeight="1">
+      <c r="G12" s="62"/>
+    </row>
+    <row r="13" spans="1:12" ht="13.5" customHeight="1">
+      <c r="G13" s="62"/>
+    </row>
+    <row r="14" spans="1:12" ht="13.5" customHeight="1">
+      <c r="G14" s="62"/>
+    </row>
+    <row r="15" spans="1:12" ht="13.5" customHeight="1">
+      <c r="G15" s="62"/>
+    </row>
+    <row r="16" spans="1:12" ht="13.5" customHeight="1">
+      <c r="G16" s="62"/>
+    </row>
+    <row r="17" spans="1:12" ht="13.5" customHeight="1">
+      <c r="G17" s="62"/>
+    </row>
+    <row r="18" spans="1:12" ht="13.5" customHeight="1">
+      <c r="G18" s="62"/>
+    </row>
+    <row r="19" spans="1:12" ht="13.5" customHeight="1">
+      <c r="G19" s="62"/>
+    </row>
+    <row r="20" spans="1:12" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A20" s="63"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="63"/>
+      <c r="J20" s="63"/>
+      <c r="K20" s="63"/>
+      <c r="L20" s="63"/>
+    </row>
+    <row r="21" spans="1:12" s="64" customFormat="1" ht="69.75" customHeight="1" thickTop="1">
+      <c r="A21" s="28" t="s">
         <v>306</v>
       </c>
-      <c r="G8" s="63"/>
-    </row>
-    <row r="9" spans="1:12" ht="13.5" customHeight="1">
-      <c r="G9" s="63"/>
-    </row>
-    <row r="10" spans="1:12" ht="13.5" customHeight="1">
-      <c r="G10" s="63"/>
-    </row>
-    <row r="11" spans="1:12" ht="13.5" customHeight="1">
-      <c r="G11" s="63"/>
-    </row>
-    <row r="12" spans="1:12" ht="13.5" customHeight="1">
-      <c r="G12" s="63"/>
-    </row>
-    <row r="13" spans="1:12" ht="13.5" customHeight="1">
-      <c r="G13" s="63"/>
-    </row>
-    <row r="14" spans="1:12" ht="13.5" customHeight="1">
-      <c r="G14" s="63"/>
-    </row>
-    <row r="15" spans="1:12" ht="13.5" customHeight="1">
-      <c r="G15" s="63"/>
-    </row>
-    <row r="16" spans="1:12" ht="13.5" customHeight="1">
-      <c r="G16" s="63"/>
-    </row>
-    <row r="17" spans="1:12" ht="13.5" customHeight="1">
-      <c r="G17" s="63"/>
-    </row>
-    <row r="18" spans="1:12" ht="13.5" customHeight="1">
-      <c r="G18" s="63"/>
-    </row>
-    <row r="19" spans="1:12" ht="13.5" customHeight="1">
-      <c r="G19" s="63"/>
-    </row>
-    <row r="20" spans="1:12" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A20" s="64"/>
-      <c r="B20" s="64"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="64"/>
-      <c r="H20" s="64"/>
-      <c r="I20" s="64"/>
-      <c r="J20" s="64"/>
-      <c r="K20" s="64"/>
-      <c r="L20" s="64"/>
-    </row>
-    <row r="21" spans="1:12" s="65" customFormat="1" ht="69.75" customHeight="1" thickTop="1">
-      <c r="A21" s="28" t="s">
+      <c r="B21" s="39" t="s">
         <v>307</v>
       </c>
-      <c r="B21" s="39" t="s">
+      <c r="C21" s="28" t="s">
         <v>308</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="D21" s="28" t="s">
         <v>309</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="E21" s="28" t="s">
         <v>310</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="F21" s="28" t="s">
         <v>311</v>
       </c>
-      <c r="F21" s="28" t="s">
+      <c r="G21" s="28" t="s">
         <v>312</v>
       </c>
-      <c r="G21" s="28" t="s">
+      <c r="H21" s="28" t="s">
         <v>313</v>
       </c>
-      <c r="H21" s="28" t="s">
+      <c r="I21" s="28" t="s">
         <v>314</v>
       </c>
-      <c r="I21" s="28" t="s">
+    </row>
+    <row r="22" spans="1:12" ht="13.5" customHeight="1">
+      <c r="A22" s="65" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A22" s="66" t="s">
+      <c r="B22" s="62" t="s">
         <v>316</v>
       </c>
-      <c r="B22" s="63" t="s">
+      <c r="C22" s="62" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="62" t="s">
         <v>317</v>
       </c>
-      <c r="C22" s="63" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="63" t="s">
+      <c r="E22" s="62" t="s">
         <v>318</v>
       </c>
-      <c r="E22" s="63" t="s">
+      <c r="F22" s="62" t="s">
         <v>319</v>
       </c>
-      <c r="F22" s="63" t="s">
+      <c r="G22" s="62" t="s">
         <v>320</v>
       </c>
-      <c r="G22" s="63" t="s">
+      <c r="H22" s="62" t="s">
+        <v>320</v>
+      </c>
+      <c r="I22" s="62" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="24.5" customHeight="1">
+      <c r="B23" s="62" t="s">
         <v>321</v>
       </c>
-      <c r="H22" s="63" t="s">
-        <v>321</v>
-      </c>
-      <c r="I22" s="63" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="24.5" customHeight="1">
-      <c r="B23" s="63" t="s">
+      <c r="C23" s="62" t="s">
         <v>322</v>
       </c>
-      <c r="C23" s="63" t="s">
+      <c r="D23" s="62" t="s">
         <v>323</v>
       </c>
-      <c r="D23" s="63" t="s">
+      <c r="E23" s="62" t="s">
         <v>324</v>
       </c>
-      <c r="E23" s="63" t="s">
+      <c r="F23" s="62" t="s">
         <v>325</v>
       </c>
-      <c r="F23" s="63" t="s">
+      <c r="G23" s="62" t="s">
         <v>326</v>
       </c>
-      <c r="G23" s="63" t="s">
+      <c r="H23" s="62" t="s">
+        <v>326</v>
+      </c>
+      <c r="I23" s="62" t="s">
         <v>327</v>
       </c>
-      <c r="H23" s="63" t="s">
-        <v>327</v>
-      </c>
-      <c r="I23" s="63" t="s">
+    </row>
+    <row r="24" spans="1:12" ht="24.5" customHeight="1">
+      <c r="B24" s="62" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" ht="24.5" customHeight="1">
-      <c r="B24" s="63" t="s">
+      <c r="C24" s="62" t="s">
         <v>329</v>
       </c>
-      <c r="C24" s="63" t="s">
+      <c r="D24" s="62" t="s">
         <v>330</v>
       </c>
-      <c r="D24" s="63" t="s">
+      <c r="F24" s="62" t="s">
         <v>331</v>
       </c>
-      <c r="F24" s="63" t="s">
+      <c r="G24" s="62" t="s">
         <v>332</v>
       </c>
-      <c r="G24" s="63" t="s">
+      <c r="H24" s="62" t="s">
+        <v>332</v>
+      </c>
+      <c r="I24" s="62" t="s">
         <v>333</v>
       </c>
-      <c r="H24" s="63" t="s">
-        <v>333</v>
-      </c>
-      <c r="I24" s="63" t="s">
+    </row>
+    <row r="25" spans="1:12" ht="13.5" customHeight="1">
+      <c r="B25" s="62" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" ht="13.5" customHeight="1">
-      <c r="B25" s="63" t="s">
+      <c r="C25" s="62" t="s">
         <v>335</v>
       </c>
-      <c r="C25" s="63" t="s">
+      <c r="D25" s="62" t="s">
         <v>336</v>
       </c>
-      <c r="D25" s="63" t="s">
+      <c r="H25" s="62" t="s">
         <v>337</v>
       </c>
-      <c r="H25" s="63" t="s">
+      <c r="I25" s="62" t="s">
         <v>338</v>
       </c>
-      <c r="I25" s="63" t="s">
+    </row>
+    <row r="26" spans="1:12" ht="13.5" customHeight="1">
+      <c r="B26" s="62" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" ht="13.5" customHeight="1">
-      <c r="B26" s="63" t="s">
+      <c r="C26" s="62" t="s">
         <v>340</v>
       </c>
-      <c r="C26" s="63" t="s">
+      <c r="H26" s="62" t="s">
         <v>341</v>
       </c>
-      <c r="H26" s="63" t="s">
+    </row>
+    <row r="27" spans="1:12" ht="13.5" customHeight="1">
+      <c r="B27" s="62" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" ht="13.5" customHeight="1">
-      <c r="B27" s="63" t="s">
+      <c r="C27" s="62" t="s">
         <v>343</v>
       </c>
-      <c r="C27" s="63" t="s">
+    </row>
+    <row r="28" spans="1:12" ht="13.5" customHeight="1">
+      <c r="B28" s="62" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" ht="13.5" customHeight="1">
-      <c r="B28" s="63" t="s">
+      <c r="C28" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="C28" s="63" t="s">
+    </row>
+    <row r="29" spans="1:12" ht="13.5" customHeight="1">
+      <c r="B29" s="62" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" ht="13.5" customHeight="1">
-      <c r="B29" s="63" t="s">
+      <c r="C29" s="62" t="s">
         <v>347</v>
       </c>
-      <c r="C29" s="63" t="s">
+    </row>
+    <row r="30" spans="1:12" ht="13.5" customHeight="1">
+      <c r="B30" s="62" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" ht="13.5" customHeight="1">
-      <c r="B30" s="63" t="s">
+      <c r="C30" s="62" t="s">
         <v>349</v>
       </c>
-      <c r="C30" s="63" t="s">
+    </row>
+    <row r="31" spans="1:12" ht="13.5" customHeight="1">
+      <c r="B31" s="62" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" ht="13.5" customHeight="1">
-      <c r="B31" s="63" t="s">
+      <c r="C31" s="62" t="s">
         <v>351</v>
       </c>
-      <c r="C31" s="63" t="s">
+    </row>
+    <row r="32" spans="1:12" ht="13.5" customHeight="1">
+      <c r="B32" s="62" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" ht="13.5" customHeight="1">
-      <c r="B32" s="63" t="s">
+      <c r="C32" s="62" t="s">
         <v>353</v>
       </c>
-      <c r="C32" s="63" t="s">
+    </row>
+    <row r="33" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B33" s="62" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="33" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B33" s="63" t="s">
+      <c r="C33" s="62" t="s">
         <v>355</v>
       </c>
-      <c r="C33" s="63" t="s">
+    </row>
+    <row r="34" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B34" s="62" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="34" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B34" s="63" t="s">
+    <row r="35" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B35" s="62" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="35" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B35" s="63" t="s">
+    <row r="36" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B36" s="62" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="36" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B36" s="63" t="s">
+    <row r="37" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B37" s="62" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="37" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B37" s="63" t="s">
+    <row r="38" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B38" s="62" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="38" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B38" s="63" t="s">
+    <row r="39" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B39" s="62" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="39" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B39" s="63" t="s">
+    <row r="40" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B40" s="62" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="40" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B40" s="63" t="s">
+    <row r="41" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B41" s="62" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="41" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B41" s="63" t="s">
+    <row r="42" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B42" s="62" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="42" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B42" s="63" t="s">
+    <row r="43" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B43" s="62" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="43" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B43" s="63" t="s">
+    <row r="44" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B44" s="62" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="44" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B44" s="63" t="s">
+    <row r="45" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B45" s="62" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="45" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B45" s="63" t="s">
+    <row r="46" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B46" s="62" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="46" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B46" s="63" t="s">
+    <row r="47" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B47" s="62" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="47" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B47" s="63" t="s">
+    <row r="48" spans="2:3" ht="13.5" customHeight="1">
+      <c r="B48" s="62" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="48" spans="2:3" ht="13.5" customHeight="1">
-      <c r="B48" s="63" t="s">
+    <row r="49" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B49" s="62" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="49" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B49" s="63" t="s">
+    <row r="50" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B50" s="62" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="50" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B50" s="63" t="s">
+    <row r="51" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B51" s="62" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="51" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B51" s="63" t="s">
+    <row r="52" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B52" s="62" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="52" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B52" s="63" t="s">
+    <row r="53" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B53" s="62" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="53" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B53" s="63" t="s">
+    <row r="54" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B54" s="62" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="54" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B54" s="63" t="s">
+    <row r="55" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B55" s="62" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="55" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B55" s="63" t="s">
+    <row r="56" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B56" s="62" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="56" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B56" s="63" t="s">
+    <row r="57" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B57" s="62" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="57" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B57" s="63" t="s">
+    <row r="58" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B58" s="62" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="58" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B58" s="63" t="s">
+    <row r="59" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B59" s="62" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="59" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B59" s="63" t="s">
+    <row r="60" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B60" s="62" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="60" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B60" s="63" t="s">
+    <row r="61" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B61" s="62" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="61" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B61" s="63" t="s">
+    <row r="62" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B62" s="62" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="62" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B62" s="63" t="s">
+    <row r="63" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B63" s="62" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="63" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B63" s="63" t="s">
+    <row r="64" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B64" s="62" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="64" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B64" s="63" t="s">
+    <row r="65" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B65" s="62" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="65" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B65" s="63" t="s">
+    <row r="66" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B66" s="62" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="66" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B66" s="63" t="s">
+    <row r="67" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B67" s="62" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="67" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B67" s="63" t="s">
+    <row r="68" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B68" s="62" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="68" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B68" s="63" t="s">
+    <row r="69" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B69" s="62" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="69" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B69" s="63" t="s">
+    <row r="70" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B70" s="62" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="70" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B70" s="63" t="s">
+    <row r="71" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B71" s="62" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="71" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B71" s="63" t="s">
+    <row r="72" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B72" s="62" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="72" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B72" s="63" t="s">
+    <row r="73" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B73" s="62" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="73" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B73" s="63" t="s">
+    <row r="74" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B74" s="62" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="74" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B74" s="63" t="s">
+    <row r="75" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B75" s="62" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="75" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B75" s="63" t="s">
+    <row r="76" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B76" s="62" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="76" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B76" s="63" t="s">
+    <row r="77" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B77" s="62" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="77" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B77" s="63" t="s">
+    <row r="78" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B78" s="62" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="78" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B78" s="63" t="s">
+    <row r="79" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B79" s="62" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="79" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B79" s="63" t="s">
+    <row r="80" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B80" s="62" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="80" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B80" s="63" t="s">
+    <row r="81" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B81" s="62" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="81" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B81" s="63" t="s">
+    <row r="82" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B82" s="62" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="82" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B82" s="63" t="s">
+    <row r="83" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B83" s="62" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="83" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B83" s="63" t="s">
+    <row r="84" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B84" s="62" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="84" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B84" s="63" t="s">
+    <row r="85" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B85" s="62" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="85" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B85" s="63" t="s">
+    <row r="86" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B86" s="62" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="86" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B86" s="63" t="s">
+    <row r="87" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B87" s="62" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="87" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B87" s="63" t="s">
+    <row r="88" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B88" s="62" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="88" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B88" s="63" t="s">
+    <row r="89" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B89" s="62" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="89" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B89" s="63" t="s">
+    <row r="90" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B90" s="62" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="90" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B90" s="63" t="s">
+    <row r="91" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B91" s="62" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="91" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B91" s="63" t="s">
+    <row r="92" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B92" s="62" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="92" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B92" s="63" t="s">
+    <row r="93" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B93" s="62" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="93" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B93" s="63" t="s">
+    <row r="94" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B94" s="62" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="94" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B94" s="63" t="s">
+    <row r="95" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B95" s="62" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="95" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B95" s="63" t="s">
+    <row r="96" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B96" s="62" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="96" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B96" s="63" t="s">
+    <row r="97" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B97" s="62" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="97" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B97" s="63" t="s">
+    <row r="98" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B98" s="62" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="98" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B98" s="63" t="s">
+    <row r="99" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B99" s="62" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="99" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B99" s="63" t="s">
+    <row r="100" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B100" s="62" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="100" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B100" s="63" t="s">
+    <row r="101" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B101" s="62" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="101" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B101" s="63" t="s">
+    <row r="102" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B102" s="62" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="102" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B102" s="63" t="s">
+    <row r="103" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B103" s="62" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="103" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B103" s="63" t="s">
+    <row r="104" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B104" s="62" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="104" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B104" s="63" t="s">
+    <row r="105" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B105" s="62" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="105" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B105" s="63" t="s">
+    <row r="106" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B106" s="62" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="106" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B106" s="63" t="s">
+    <row r="107" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B107" s="62" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="107" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B107" s="63" t="s">
+    <row r="108" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B108" s="62" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="108" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B108" s="63" t="s">
+    <row r="109" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B109" s="62" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="109" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B109" s="63" t="s">
+    <row r="110" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B110" s="62" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="110" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B110" s="63" t="s">
+    <row r="111" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B111" s="62" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="111" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B111" s="63" t="s">
+    <row r="112" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B112" s="62" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="112" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B112" s="63" t="s">
+    <row r="113" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B113" s="62" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="113" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B113" s="63" t="s">
+    <row r="114" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B114" s="62" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="114" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B114" s="63" t="s">
+    <row r="115" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B115" s="62" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="115" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B115" s="63" t="s">
+    <row r="116" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B116" s="62" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="116" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B116" s="63" t="s">
+    <row r="117" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B117" s="62" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="117" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B117" s="63" t="s">
+    <row r="118" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B118" s="62" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="118" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B118" s="63" t="s">
+    <row r="119" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B119" s="62" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="119" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B119" s="63" t="s">
+    <row r="120" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B120" s="62" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="120" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B120" s="63" t="s">
+    <row r="121" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B121" s="62" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="121" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B121" s="63" t="s">
+    <row r="122" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B122" s="62" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="122" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B122" s="63" t="s">
+    <row r="123" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B123" s="62" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="123" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B123" s="63" t="s">
+    <row r="124" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B124" s="62" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="124" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B124" s="63" t="s">
+    <row r="125" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B125" s="62" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="125" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B125" s="63" t="s">
+    <row r="126" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B126" s="62" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="126" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B126" s="63" t="s">
+    <row r="127" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B127" s="62" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="127" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B127" s="63" t="s">
+    <row r="128" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B128" s="62" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="128" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B128" s="63" t="s">
+    <row r="129" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B129" s="62" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="129" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B129" s="63" t="s">
+    <row r="130" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B130" s="62" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="130" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B130" s="63" t="s">
+    <row r="131" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B131" s="62" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="131" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B131" s="63" t="s">
+    <row r="132" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B132" s="62" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="132" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B132" s="63" t="s">
+    <row r="133" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B133" s="62" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="133" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B133" s="63" t="s">
+    <row r="134" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B134" s="62" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="134" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B134" s="63" t="s">
+    <row r="135" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B135" s="62" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="135" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B135" s="63" t="s">
+    <row r="136" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B136" s="62" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="136" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B136" s="63" t="s">
+    <row r="137" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B137" s="62" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="137" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B137" s="63" t="s">
+    <row r="138" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B138" s="62" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="138" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B138" s="63" t="s">
+    <row r="139" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B139" s="62" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="139" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B139" s="63" t="s">
+    <row r="140" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B140" s="62" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="140" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B140" s="63" t="s">
+    <row r="141" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B141" s="62" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="141" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B141" s="63" t="s">
+    <row r="142" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B142" s="62" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="142" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B142" s="63" t="s">
+    <row r="143" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B143" s="62" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="143" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B143" s="63" t="s">
+    <row r="144" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B144" s="62" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="144" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B144" s="63" t="s">
+    <row r="145" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B145" s="62" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="145" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B145" s="63" t="s">
+    <row r="146" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B146" s="62" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="146" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B146" s="63" t="s">
+    <row r="147" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B147" s="62" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="147" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B147" s="63" t="s">
+    <row r="148" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B148" s="62" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="148" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B148" s="63" t="s">
+    <row r="149" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B149" s="62" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="149" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B149" s="63" t="s">
+    <row r="150" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B150" s="62" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="150" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B150" s="63" t="s">
+    <row r="151" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B151" s="62" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="151" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B151" s="63" t="s">
+    <row r="152" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B152" s="62" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="152" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B152" s="63" t="s">
+    <row r="153" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B153" s="62" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="153" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B153" s="63" t="s">
+    <row r="154" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B154" s="62" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="154" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B154" s="63" t="s">
+    <row r="155" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B155" s="62" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="155" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B155" s="63" t="s">
+    <row r="156" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B156" s="62" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="156" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B156" s="63" t="s">
+    <row r="157" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B157" s="62" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="157" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B157" s="63" t="s">
+    <row r="158" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B158" s="62" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="158" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B158" s="63" t="s">
+    <row r="159" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B159" s="62" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="159" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B159" s="63" t="s">
+    <row r="160" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B160" s="62" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="160" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B160" s="63" t="s">
+    <row r="161" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B161" s="62" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="161" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B161" s="63" t="s">
+    <row r="162" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B162" s="62" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="162" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B162" s="63" t="s">
+    <row r="163" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B163" s="62" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="163" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B163" s="63" t="s">
+    <row r="164" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B164" s="62" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="164" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B164" s="63" t="s">
+    <row r="165" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B165" s="62" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="165" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B165" s="63" t="s">
+    <row r="166" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B166" s="62" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="166" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B166" s="63" t="s">
+    <row r="167" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B167" s="62" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="167" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B167" s="63" t="s">
+    <row r="168" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B168" s="62" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="168" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B168" s="63" t="s">
+    <row r="169" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B169" s="62" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="169" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B169" s="63" t="s">
+    <row r="170" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B170" s="62" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="170" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B170" s="63" t="s">
+    <row r="171" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B171" s="62" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="171" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B171" s="63" t="s">
+    <row r="172" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B172" s="62" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="172" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B172" s="63" t="s">
+    <row r="173" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B173" s="62" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="173" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B173" s="63" t="s">
+    <row r="174" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B174" s="62" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="174" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B174" s="63" t="s">
+    <row r="175" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B175" s="62" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="175" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B175" s="63" t="s">
+    <row r="176" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B176" s="62" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="176" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B176" s="63" t="s">
+    <row r="177" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B177" s="62" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="177" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B177" s="63" t="s">
+    <row r="178" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B178" s="62" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="178" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B178" s="63" t="s">
+    <row r="179" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B179" s="62" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="179" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B179" s="63" t="s">
+    <row r="180" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B180" s="62" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="180" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B180" s="63" t="s">
+    <row r="181" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B181" s="62" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="181" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B181" s="63" t="s">
+    <row r="182" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B182" s="62" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="182" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B182" s="63" t="s">
+    <row r="183" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B183" s="62" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="183" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B183" s="63" t="s">
+    <row r="184" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B184" s="62" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="184" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B184" s="63" t="s">
+    <row r="185" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B185" s="62" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="185" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B185" s="63" t="s">
+    <row r="186" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B186" s="62" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="186" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B186" s="63" t="s">
+    <row r="187" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B187" s="62" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="187" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B187" s="63" t="s">
+    <row r="188" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B188" s="62" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="188" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B188" s="63" t="s">
+    <row r="189" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B189" s="62" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="189" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B189" s="63" t="s">
+    <row r="190" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B190" s="62" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="190" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B190" s="63" t="s">
+    <row r="191" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B191" s="62" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="191" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B191" s="63" t="s">
+    <row r="192" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B192" s="62" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="192" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B192" s="63" t="s">
+    <row r="193" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B193" s="62" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="193" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B193" s="63" t="s">
+    <row r="194" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B194" s="62" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="194" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B194" s="63" t="s">
+    <row r="195" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B195" s="62" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="195" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B195" s="63" t="s">
+    <row r="196" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B196" s="62" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="196" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B196" s="63" t="s">
+    <row r="197" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B197" s="62" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="197" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B197" s="63" t="s">
+    <row r="198" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B198" s="62" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="198" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B198" s="63" t="s">
+    <row r="199" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B199" s="62" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="199" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B199" s="63" t="s">
+    <row r="200" spans="2:2" ht="13.5" customHeight="1">
+      <c r="B200" s="62" t="s">
         <v>522</v>
-      </c>
-    </row>
-    <row r="200" spans="2:2" ht="13.5" customHeight="1">
-      <c r="B200" s="63" t="s">
-        <v>523</v>
       </c>
     </row>
   </sheetData>
@@ -4895,7 +4767,7 @@
   <dimension ref="A1:Y85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5104,7 +4976,7 @@
         <v>183</v>
       </c>
       <c r="D4" s="49" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E4" s="36" t="s">
         <v>160</v>
@@ -5146,7 +5018,7 @@
         <v>181</v>
       </c>
       <c r="D5" s="49" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E5" s="36" t="s">
         <v>169</v>
@@ -5188,7 +5060,7 @@
         <v>182</v>
       </c>
       <c r="D6" s="49" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E6" s="36" t="s">
         <v>173</v>
@@ -5230,7 +5102,7 @@
         <v>184</v>
       </c>
       <c r="D7" s="49" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E7" s="36" t="s">
         <v>164</v>
@@ -5842,7 +5714,7 @@
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" ht="24.5" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -5856,50 +5728,50 @@
     </row>
     <row r="4" spans="1:3" ht="13.5" customHeight="1">
       <c r="A4" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="B4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A5" s="67" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A5" s="68" t="s">
+      <c r="B5" s="67" t="s">
         <v>553</v>
       </c>
-      <c r="B5" s="68" t="s">
+    </row>
+    <row r="6" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A6" s="67" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="67" t="s">
         <v>554</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A6" s="68" t="s">
-        <v>107</v>
-      </c>
-      <c r="B6" s="68" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="13.5" customHeight="1">
       <c r="A7" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>556</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="13.5" customHeight="1">
       <c r="A8" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>558</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="13.5" customHeight="1">
       <c r="A9" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>560</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>561</v>
       </c>
     </row>
   </sheetData>
@@ -5941,7 +5813,7 @@
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" ht="18" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -5958,23 +5830,23 @@
         <v>105</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="13.5" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="13.5" customHeight="1">
       <c r="A6" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>565</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="13.5" customHeight="1">
@@ -5987,18 +5859,18 @@
     </row>
     <row r="8" spans="1:3" ht="13.5" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="13.5" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="13.5" customHeight="1">
@@ -6006,7 +5878,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
   </sheetData>
@@ -6027,7 +5899,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6207,8 +6079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ6"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6301,8 +6173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE28"/>
   <sheetViews>
-    <sheetView topLeftCell="L2" workbookViewId="0">
-      <selection activeCell="AD4" sqref="AD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6440,11 +6312,11 @@
       <c r="M2" s="25"/>
       <c r="N2" s="25"/>
       <c r="O2" s="25"/>
-      <c r="P2" s="53" t="s">
+      <c r="P2" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="53"/>
+      <c r="Q2" s="68"/>
+      <c r="R2" s="68"/>
       <c r="Z2" s="25"/>
       <c r="AC2" s="26"/>
       <c r="AD2" s="26"/>
@@ -6553,10 +6425,10 @@
         <v>209</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F4" s="15" t="s">
         <v>109</v>
@@ -6626,7 +6498,7 @@
     </row>
     <row r="5" spans="1:31" ht="13.5" customHeight="1">
       <c r="A5" s="19" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>210</v>
@@ -6638,7 +6510,7 @@
         <v>210</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F5" s="15" t="s">
         <v>109</v>
@@ -6715,7 +6587,7 @@
         <v>213</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>90</v>
@@ -7119,13 +6991,13 @@
         <v>226</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>227</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>90</v>
@@ -7453,7 +7325,7 @@
         <v>238</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>90</v>
@@ -7535,7 +7407,7 @@
         <v>239</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>90</v>
@@ -7617,7 +7489,7 @@
         <v>242</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>90</v>
@@ -8017,19 +7889,19 @@
       <c r="AD21" s="33"/>
     </row>
     <row r="22" spans="1:31">
-      <c r="A22" s="54" t="s">
+      <c r="A22" s="53" t="s">
         <v>255</v>
       </c>
-      <c r="B22" s="54" t="s">
+      <c r="B22" s="53" t="s">
         <v>254</v>
       </c>
-      <c r="C22" s="55" t="s">
-        <v>256</v>
-      </c>
-      <c r="D22" s="56" t="s">
+      <c r="C22" s="54" t="s">
+        <v>569</v>
+      </c>
+      <c r="D22" s="55" t="s">
         <v>254</v>
       </c>
-      <c r="E22" s="56" t="s">
+      <c r="E22" s="55" t="s">
         <v>90</v>
       </c>
       <c r="F22" s="15" t="s">
@@ -8038,81 +7910,81 @@
       <c r="G22" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="H22" s="57">
-        <v>0</v>
-      </c>
-      <c r="I22" s="56" t="s">
+      <c r="H22" s="56">
+        <v>0</v>
+      </c>
+      <c r="I22" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="J22" s="58" t="s">
+      <c r="J22" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="K22" s="54">
+      <c r="K22" s="53">
         <v>2</v>
       </c>
-      <c r="L22" s="59">
+      <c r="L22" s="58">
         <v>7</v>
       </c>
-      <c r="M22" s="59">
-        <v>0</v>
-      </c>
-      <c r="N22" s="59">
+      <c r="M22" s="58">
+        <v>0</v>
+      </c>
+      <c r="N22" s="58">
         <v>1000000000</v>
       </c>
-      <c r="O22" s="59">
-        <v>0</v>
-      </c>
-      <c r="P22" s="60">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="60">
+      <c r="O22" s="58">
+        <v>0</v>
+      </c>
+      <c r="P22" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="59">
         <v>2</v>
       </c>
-      <c r="R22" s="60">
-        <v>0</v>
-      </c>
-      <c r="S22" s="54">
+      <c r="R22" s="59">
+        <v>0</v>
+      </c>
+      <c r="S22" s="53">
         <v>10</v>
       </c>
-      <c r="T22" s="54">
+      <c r="T22" s="53">
         <v>7.5</v>
       </c>
-      <c r="U22" s="54">
+      <c r="U22" s="53">
         <v>14</v>
       </c>
-      <c r="V22" s="54">
+      <c r="V22" s="53">
         <v>1</v>
       </c>
-      <c r="W22" s="56"/>
-      <c r="X22" s="61"/>
-      <c r="Y22" s="61"/>
-      <c r="Z22" s="59">
+      <c r="W22" s="55"/>
+      <c r="X22" s="60"/>
+      <c r="Y22" s="60"/>
+      <c r="Z22" s="58">
         <v>10</v>
       </c>
-      <c r="AA22" s="60">
-        <v>0</v>
-      </c>
-      <c r="AB22" s="60">
-        <v>0</v>
-      </c>
-      <c r="AC22" s="61"/>
-      <c r="AD22" s="61"/>
-      <c r="AE22" s="55"/>
+      <c r="AA22" s="59">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="59">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="60"/>
+      <c r="AD22" s="60"/>
+      <c r="AE22" s="54"/>
     </row>
     <row r="23" spans="1:31">
-      <c r="A23" s="54" t="s">
+      <c r="A23" s="53" t="s">
+        <v>256</v>
+      </c>
+      <c r="B23" s="53" t="s">
         <v>257</v>
       </c>
-      <c r="B23" s="54" t="s">
+      <c r="C23" s="54" t="s">
         <v>258</v>
       </c>
-      <c r="C23" s="55" t="s">
-        <v>259</v>
-      </c>
-      <c r="D23" s="56" t="s">
-        <v>258</v>
-      </c>
-      <c r="E23" s="56" t="s">
+      <c r="D23" s="55" t="s">
+        <v>257</v>
+      </c>
+      <c r="E23" s="55" t="s">
         <v>90</v>
       </c>
       <c r="F23" s="15" t="s">
@@ -8121,81 +7993,81 @@
       <c r="G23" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="H23" s="57">
-        <v>0</v>
-      </c>
-      <c r="I23" s="56" t="s">
+      <c r="H23" s="56">
+        <v>0</v>
+      </c>
+      <c r="I23" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="J23" s="58" t="s">
+      <c r="J23" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="K23" s="54">
+      <c r="K23" s="53">
         <v>2</v>
       </c>
-      <c r="L23" s="59">
+      <c r="L23" s="58">
         <v>7</v>
       </c>
-      <c r="M23" s="59">
-        <v>0</v>
-      </c>
-      <c r="N23" s="59">
+      <c r="M23" s="58">
+        <v>0</v>
+      </c>
+      <c r="N23" s="58">
         <v>1000000000</v>
       </c>
-      <c r="O23" s="59">
-        <v>0</v>
-      </c>
-      <c r="P23" s="60">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="60">
+      <c r="O23" s="58">
+        <v>0</v>
+      </c>
+      <c r="P23" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="59">
         <v>2</v>
       </c>
-      <c r="R23" s="60">
-        <v>0</v>
-      </c>
-      <c r="S23" s="54">
+      <c r="R23" s="59">
+        <v>0</v>
+      </c>
+      <c r="S23" s="53">
         <v>10</v>
       </c>
-      <c r="T23" s="54">
+      <c r="T23" s="53">
         <v>7.5</v>
       </c>
-      <c r="U23" s="54">
+      <c r="U23" s="53">
         <v>14</v>
       </c>
-      <c r="V23" s="54">
+      <c r="V23" s="53">
         <v>1</v>
       </c>
-      <c r="W23" s="56"/>
-      <c r="X23" s="61"/>
-      <c r="Y23" s="61"/>
-      <c r="Z23" s="59">
+      <c r="W23" s="55"/>
+      <c r="X23" s="60"/>
+      <c r="Y23" s="60"/>
+      <c r="Z23" s="58">
         <v>10</v>
       </c>
-      <c r="AA23" s="60">
-        <v>0</v>
-      </c>
-      <c r="AB23" s="60">
-        <v>0</v>
-      </c>
-      <c r="AC23" s="61"/>
-      <c r="AD23" s="61"/>
-      <c r="AE23" s="55"/>
+      <c r="AA23" s="59">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="59">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="60"/>
+      <c r="AD23" s="60"/>
+      <c r="AE23" s="54"/>
     </row>
     <row r="24" spans="1:31">
-      <c r="A24" s="54" t="s">
-        <v>261</v>
-      </c>
-      <c r="B24" s="54" t="s">
-        <v>261</v>
-      </c>
-      <c r="C24" s="55" t="s">
+      <c r="A24" s="53" t="s">
         <v>260</v>
       </c>
-      <c r="D24" s="56" t="s">
-        <v>544</v>
-      </c>
-      <c r="E24" s="56" t="s">
+      <c r="B24" s="53" t="s">
+        <v>260</v>
+      </c>
+      <c r="C24" s="54" t="s">
+        <v>259</v>
+      </c>
+      <c r="D24" s="55" t="s">
+        <v>543</v>
+      </c>
+      <c r="E24" s="55" t="s">
         <v>90</v>
       </c>
       <c r="F24" s="15" t="s">
@@ -8204,81 +8076,81 @@
       <c r="G24" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="H24" s="57">
-        <v>0</v>
-      </c>
-      <c r="I24" s="56" t="s">
+      <c r="H24" s="56">
+        <v>0</v>
+      </c>
+      <c r="I24" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="J24" s="58" t="s">
+      <c r="J24" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="K24" s="54">
+      <c r="K24" s="53">
         <v>2</v>
       </c>
-      <c r="L24" s="59">
+      <c r="L24" s="58">
         <v>7</v>
       </c>
-      <c r="M24" s="59">
-        <v>0</v>
-      </c>
-      <c r="N24" s="59">
+      <c r="M24" s="58">
+        <v>0</v>
+      </c>
+      <c r="N24" s="58">
         <v>1000000000</v>
       </c>
-      <c r="O24" s="59">
-        <v>0</v>
-      </c>
-      <c r="P24" s="60">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="60">
+      <c r="O24" s="58">
+        <v>0</v>
+      </c>
+      <c r="P24" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="59">
         <v>2</v>
       </c>
-      <c r="R24" s="60">
-        <v>0</v>
-      </c>
-      <c r="S24" s="54">
+      <c r="R24" s="59">
+        <v>0</v>
+      </c>
+      <c r="S24" s="53">
         <v>10</v>
       </c>
-      <c r="T24" s="54">
+      <c r="T24" s="53">
         <v>7.5</v>
       </c>
-      <c r="U24" s="54">
+      <c r="U24" s="53">
         <v>14</v>
       </c>
-      <c r="V24" s="54">
+      <c r="V24" s="53">
         <v>1</v>
       </c>
-      <c r="W24" s="56"/>
-      <c r="X24" s="61"/>
-      <c r="Y24" s="61"/>
-      <c r="Z24" s="59">
+      <c r="W24" s="55"/>
+      <c r="X24" s="60"/>
+      <c r="Y24" s="60"/>
+      <c r="Z24" s="58">
         <v>10</v>
       </c>
-      <c r="AA24" s="60">
-        <v>0</v>
-      </c>
-      <c r="AB24" s="60">
-        <v>0</v>
-      </c>
-      <c r="AC24" s="61"/>
-      <c r="AD24" s="61"/>
-      <c r="AE24" s="55"/>
+      <c r="AA24" s="59">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="59">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="60"/>
+      <c r="AD24" s="60"/>
+      <c r="AE24" s="54"/>
     </row>
     <row r="25" spans="1:31">
-      <c r="A25" s="54" t="s">
+      <c r="A25" s="53" t="s">
+        <v>261</v>
+      </c>
+      <c r="B25" s="53" t="s">
         <v>262</v>
       </c>
-      <c r="B25" s="54" t="s">
+      <c r="C25" s="54" t="s">
         <v>263</v>
       </c>
-      <c r="C25" s="55" t="s">
-        <v>264</v>
-      </c>
-      <c r="D25" s="56" t="s">
-        <v>263</v>
-      </c>
-      <c r="E25" s="56" t="s">
+      <c r="D25" s="55" t="s">
+        <v>262</v>
+      </c>
+      <c r="E25" s="55" t="s">
         <v>90</v>
       </c>
       <c r="F25" s="15" t="s">
@@ -8287,81 +8159,81 @@
       <c r="G25" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="H25" s="57">
-        <v>0</v>
-      </c>
-      <c r="I25" s="56" t="s">
+      <c r="H25" s="56">
+        <v>0</v>
+      </c>
+      <c r="I25" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="J25" s="58" t="s">
+      <c r="J25" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="K25" s="54">
+      <c r="K25" s="53">
         <v>2</v>
       </c>
-      <c r="L25" s="59">
+      <c r="L25" s="58">
         <v>7</v>
       </c>
-      <c r="M25" s="59">
-        <v>0</v>
-      </c>
-      <c r="N25" s="59">
+      <c r="M25" s="58">
+        <v>0</v>
+      </c>
+      <c r="N25" s="58">
         <v>1000000000</v>
       </c>
-      <c r="O25" s="59">
-        <v>0</v>
-      </c>
-      <c r="P25" s="60">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="60">
+      <c r="O25" s="58">
+        <v>0</v>
+      </c>
+      <c r="P25" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="59">
         <v>2</v>
       </c>
-      <c r="R25" s="60">
-        <v>0</v>
-      </c>
-      <c r="S25" s="54">
+      <c r="R25" s="59">
+        <v>0</v>
+      </c>
+      <c r="S25" s="53">
         <v>10</v>
       </c>
-      <c r="T25" s="54">
+      <c r="T25" s="53">
         <v>7.5</v>
       </c>
-      <c r="U25" s="54">
+      <c r="U25" s="53">
         <v>14</v>
       </c>
-      <c r="V25" s="54">
+      <c r="V25" s="53">
         <v>1</v>
       </c>
-      <c r="W25" s="56"/>
-      <c r="X25" s="61"/>
-      <c r="Y25" s="61"/>
-      <c r="Z25" s="59">
+      <c r="W25" s="55"/>
+      <c r="X25" s="60"/>
+      <c r="Y25" s="60"/>
+      <c r="Z25" s="58">
         <v>10</v>
       </c>
-      <c r="AA25" s="60">
-        <v>0</v>
-      </c>
-      <c r="AB25" s="60">
-        <v>0</v>
-      </c>
-      <c r="AC25" s="61"/>
-      <c r="AD25" s="61"/>
-      <c r="AE25" s="55"/>
+      <c r="AA25" s="59">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="59">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="60"/>
+      <c r="AD25" s="60"/>
+      <c r="AE25" s="54"/>
     </row>
     <row r="26" spans="1:31">
-      <c r="A26" s="54" t="s">
+      <c r="A26" s="53" t="s">
+        <v>264</v>
+      </c>
+      <c r="B26" s="53" t="s">
+        <v>264</v>
+      </c>
+      <c r="C26" s="54" t="s">
         <v>265</v>
       </c>
-      <c r="B26" s="54" t="s">
-        <v>265</v>
-      </c>
-      <c r="C26" s="55" t="s">
-        <v>266</v>
-      </c>
-      <c r="D26" s="56" t="s">
-        <v>545</v>
-      </c>
-      <c r="E26" s="56" t="s">
+      <c r="D26" s="55" t="s">
+        <v>544</v>
+      </c>
+      <c r="E26" s="55" t="s">
         <v>90</v>
       </c>
       <c r="F26" s="15" t="s">
@@ -8370,81 +8242,81 @@
       <c r="G26" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="H26" s="57">
-        <v>0</v>
-      </c>
-      <c r="I26" s="56" t="s">
+      <c r="H26" s="56">
+        <v>0</v>
+      </c>
+      <c r="I26" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="J26" s="58" t="s">
+      <c r="J26" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="K26" s="54">
+      <c r="K26" s="53">
         <v>2</v>
       </c>
-      <c r="L26" s="59">
+      <c r="L26" s="58">
         <v>7</v>
       </c>
-      <c r="M26" s="59">
-        <v>0</v>
-      </c>
-      <c r="N26" s="59">
+      <c r="M26" s="58">
+        <v>0</v>
+      </c>
+      <c r="N26" s="58">
         <v>1000000000</v>
       </c>
-      <c r="O26" s="59">
-        <v>0</v>
-      </c>
-      <c r="P26" s="60">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="60">
+      <c r="O26" s="58">
+        <v>0</v>
+      </c>
+      <c r="P26" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="59">
         <v>2</v>
       </c>
-      <c r="R26" s="60">
-        <v>0</v>
-      </c>
-      <c r="S26" s="54">
+      <c r="R26" s="59">
+        <v>0</v>
+      </c>
+      <c r="S26" s="53">
         <v>10</v>
       </c>
-      <c r="T26" s="54">
+      <c r="T26" s="53">
         <v>7.5</v>
       </c>
-      <c r="U26" s="54">
+      <c r="U26" s="53">
         <v>14</v>
       </c>
-      <c r="V26" s="54">
+      <c r="V26" s="53">
         <v>1</v>
       </c>
-      <c r="W26" s="56"/>
-      <c r="X26" s="61"/>
-      <c r="Y26" s="61"/>
-      <c r="Z26" s="59">
+      <c r="W26" s="55"/>
+      <c r="X26" s="60"/>
+      <c r="Y26" s="60"/>
+      <c r="Z26" s="58">
         <v>10</v>
       </c>
-      <c r="AA26" s="60">
-        <v>0</v>
-      </c>
-      <c r="AB26" s="60">
-        <v>0</v>
-      </c>
-      <c r="AC26" s="61"/>
-      <c r="AD26" s="61"/>
-      <c r="AE26" s="55"/>
+      <c r="AA26" s="59">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="59">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="60"/>
+      <c r="AD26" s="60"/>
+      <c r="AE26" s="54"/>
     </row>
     <row r="27" spans="1:31">
-      <c r="A27" s="54" t="s">
+      <c r="A27" s="53" t="s">
+        <v>266</v>
+      </c>
+      <c r="B27" s="53" t="s">
         <v>267</v>
       </c>
-      <c r="B27" s="54" t="s">
+      <c r="C27" s="54" t="s">
         <v>268</v>
       </c>
-      <c r="C27" s="55" t="s">
-        <v>269</v>
-      </c>
-      <c r="D27" s="56" t="s">
-        <v>268</v>
-      </c>
-      <c r="E27" s="56" t="s">
+      <c r="D27" s="55" t="s">
+        <v>267</v>
+      </c>
+      <c r="E27" s="55" t="s">
         <v>90</v>
       </c>
       <c r="F27" s="15" t="s">
@@ -8453,81 +8325,81 @@
       <c r="G27" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="H27" s="57">
-        <v>0</v>
-      </c>
-      <c r="I27" s="56" t="s">
+      <c r="H27" s="56">
+        <v>0</v>
+      </c>
+      <c r="I27" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="J27" s="58" t="s">
+      <c r="J27" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="K27" s="54">
+      <c r="K27" s="53">
         <v>2</v>
       </c>
-      <c r="L27" s="59">
+      <c r="L27" s="58">
         <v>7</v>
       </c>
-      <c r="M27" s="59">
-        <v>0</v>
-      </c>
-      <c r="N27" s="59">
+      <c r="M27" s="58">
+        <v>0</v>
+      </c>
+      <c r="N27" s="58">
         <v>1000000000</v>
       </c>
-      <c r="O27" s="59">
-        <v>0</v>
-      </c>
-      <c r="P27" s="60">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="60">
+      <c r="O27" s="58">
+        <v>0</v>
+      </c>
+      <c r="P27" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="59">
         <v>2</v>
       </c>
-      <c r="R27" s="60">
-        <v>0</v>
-      </c>
-      <c r="S27" s="54">
+      <c r="R27" s="59">
+        <v>0</v>
+      </c>
+      <c r="S27" s="53">
         <v>10</v>
       </c>
-      <c r="T27" s="54">
+      <c r="T27" s="53">
         <v>7.5</v>
       </c>
-      <c r="U27" s="54">
+      <c r="U27" s="53">
         <v>14</v>
       </c>
-      <c r="V27" s="54">
+      <c r="V27" s="53">
         <v>1</v>
       </c>
-      <c r="W27" s="56"/>
-      <c r="X27" s="61"/>
-      <c r="Y27" s="61"/>
-      <c r="Z27" s="59">
+      <c r="W27" s="55"/>
+      <c r="X27" s="60"/>
+      <c r="Y27" s="60"/>
+      <c r="Z27" s="58">
         <v>10</v>
       </c>
-      <c r="AA27" s="60">
-        <v>0</v>
-      </c>
-      <c r="AB27" s="60">
-        <v>0</v>
-      </c>
-      <c r="AC27" s="61"/>
-      <c r="AD27" s="61"/>
-      <c r="AE27" s="55"/>
+      <c r="AA27" s="59">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="59">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="60"/>
+      <c r="AD27" s="60"/>
+      <c r="AE27" s="54"/>
     </row>
     <row r="28" spans="1:31">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="53" t="s">
+        <v>270</v>
+      </c>
+      <c r="B28" s="53" t="s">
+        <v>269</v>
+      </c>
+      <c r="C28" s="54" t="s">
         <v>271</v>
       </c>
-      <c r="B28" s="54" t="s">
-        <v>270</v>
-      </c>
-      <c r="C28" s="55" t="s">
-        <v>272</v>
-      </c>
-      <c r="D28" s="56" t="s">
-        <v>270</v>
-      </c>
-      <c r="E28" s="56" t="s">
+      <c r="D28" s="55" t="s">
+        <v>269</v>
+      </c>
+      <c r="E28" s="55" t="s">
         <v>90</v>
       </c>
       <c r="F28" s="15" t="s">
@@ -8536,66 +8408,66 @@
       <c r="G28" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="H28" s="57">
-        <v>0</v>
-      </c>
-      <c r="I28" s="56" t="s">
+      <c r="H28" s="56">
+        <v>0</v>
+      </c>
+      <c r="I28" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="J28" s="58" t="s">
+      <c r="J28" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="K28" s="54">
+      <c r="K28" s="53">
         <v>2</v>
       </c>
-      <c r="L28" s="59">
+      <c r="L28" s="58">
         <v>7</v>
       </c>
-      <c r="M28" s="59">
-        <v>0</v>
-      </c>
-      <c r="N28" s="59">
+      <c r="M28" s="58">
+        <v>0</v>
+      </c>
+      <c r="N28" s="58">
         <v>1000000000</v>
       </c>
-      <c r="O28" s="59">
-        <v>0</v>
-      </c>
-      <c r="P28" s="60">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="60">
+      <c r="O28" s="58">
+        <v>0</v>
+      </c>
+      <c r="P28" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="59">
         <v>2</v>
       </c>
-      <c r="R28" s="60">
-        <v>0</v>
-      </c>
-      <c r="S28" s="54">
+      <c r="R28" s="59">
+        <v>0</v>
+      </c>
+      <c r="S28" s="53">
         <v>10</v>
       </c>
-      <c r="T28" s="54">
+      <c r="T28" s="53">
         <v>7.5</v>
       </c>
-      <c r="U28" s="54">
+      <c r="U28" s="53">
         <v>14</v>
       </c>
-      <c r="V28" s="54">
+      <c r="V28" s="53">
         <v>1</v>
       </c>
-      <c r="W28" s="56"/>
-      <c r="X28" s="61"/>
-      <c r="Y28" s="61"/>
-      <c r="Z28" s="59">
+      <c r="W28" s="55"/>
+      <c r="X28" s="60"/>
+      <c r="Y28" s="60"/>
+      <c r="Z28" s="58">
         <v>10</v>
       </c>
-      <c r="AA28" s="60">
-        <v>0</v>
-      </c>
-      <c r="AB28" s="60">
-        <v>0</v>
-      </c>
-      <c r="AC28" s="61"/>
-      <c r="AD28" s="61"/>
-      <c r="AE28" s="55"/>
+      <c r="AA28" s="59">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="59">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="60"/>
+      <c r="AD28" s="60"/>
+      <c r="AE28" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8620,7 +8492,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="167" yWindow="253" count="13">
@@ -8714,15 +8585,6 @@
           </x14:formula2>
           <xm:sqref>H4:H21</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" operator="equal" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Select a valid entry from the drop-down menu" promptTitle="Field or Lab analysis?" prompt="Select a valid entry from the drop-down menu">
-          <x14:formula1>
-            <xm:f>[1]Constants!#REF!</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>E4:E21</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Select a valid entry from the drop-down menu" promptTitle="Valid categories" prompt="Select a valid entry from the drop-down menu">
           <x14:formula1>
             <xm:f>'Analysis Categories'!$A$4:$A$44</xm:f>
@@ -8734,6 +8596,12 @@
             <xm:f>'Lab Departments'!$A$4:$A$49</xm:f>
           </x14:formula1>
           <xm:sqref>G4:G28</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" operator="equal" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Select a valid entry from the drop-down menu" promptTitle="Field or Lab analysis?" prompt="Select a valid entry from the drop-down menu">
+          <x14:formula1>
+            <xm:f>Constants!$K$2:$K$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>E4:E28</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -8813,7 +8681,7 @@
     <row r="4" spans="1:15" ht="13.5" customHeight="1">
       <c r="A4" s="14"/>
       <c r="B4" s="17" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>198</v>
@@ -8843,7 +8711,7 @@
         <v>203</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="13.5" customHeight="1">
@@ -8897,7 +8765,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8933,7 +8801,7 @@
     </row>
     <row r="4" spans="1:3" s="12" customFormat="1" ht="12.25" customHeight="1">
       <c r="A4" s="14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>224</v>
@@ -8941,7 +8809,7 @@
     </row>
     <row r="5" spans="1:3" ht="13.5" customHeight="1">
       <c r="A5" s="14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>218</v>
@@ -8949,7 +8817,7 @@
     </row>
     <row r="6" spans="1:3" ht="13.5" customHeight="1">
       <c r="A6" s="14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>215</v>
@@ -8957,7 +8825,7 @@
     </row>
     <row r="7" spans="1:3" ht="13.5" customHeight="1">
       <c r="A7" s="14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>237</v>
@@ -8965,7 +8833,7 @@
     </row>
     <row r="8" spans="1:3" ht="13.5" customHeight="1">
       <c r="A8" s="14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>226</v>
@@ -8973,7 +8841,7 @@
     </row>
     <row r="9" spans="1:3" ht="13.5" customHeight="1">
       <c r="A9" s="14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>231</v>
@@ -8981,7 +8849,7 @@
     </row>
     <row r="10" spans="1:3" ht="13.5" customHeight="1">
       <c r="A10" s="14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>221</v>
@@ -8989,7 +8857,7 @@
     </row>
     <row r="11" spans="1:3" ht="13.5" customHeight="1">
       <c r="A11" s="14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>212</v>
@@ -8997,7 +8865,7 @@
     </row>
     <row r="12" spans="1:3" ht="13.5" customHeight="1">
       <c r="A12" s="14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>218</v>
@@ -9005,7 +8873,7 @@
     </row>
     <row r="13" spans="1:3" ht="13.5" customHeight="1">
       <c r="A13" s="14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>234</v>
@@ -9013,15 +8881,15 @@
     </row>
     <row r="14" spans="1:3" ht="13.5" customHeight="1">
       <c r="A14" s="14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="13.5" customHeight="1">
       <c r="A15" s="14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>207</v>
@@ -9048,7 +8916,7 @@
         <v>204</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="13.5" customHeight="1">
@@ -9056,7 +8924,7 @@
         <v>204</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="13.5" customHeight="1">
@@ -9064,7 +8932,7 @@
         <v>204</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="13.5" customHeight="1">
@@ -9072,7 +8940,7 @@
         <v>204</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="13.5" customHeight="1">
@@ -9080,7 +8948,7 @@
         <v>204</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -9104,7 +8972,7 @@
         <v>202</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -9128,7 +8996,6 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">

</xml_diff>